<commit_message>
Pre-travail avant réunion 1/04
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ADAVEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC5EE434-DE4F-4225-800B-15F6D207029E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8048C047-CE91-423B-8BB5-82CB8F08B1D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="179">
   <si>
     <t>ID</t>
   </si>
@@ -554,6 +554,9 @@
   </si>
   <si>
     <t>Road</t>
+  </si>
+  <si>
+    <t>Order</t>
   </si>
 </sst>
 </file>
@@ -669,7 +672,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -753,11 +756,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,9 +968,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -939,59 +997,39 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,14 +1050,65 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1027,6 +1116,414 @@
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Roboto"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BC2E6"/>
+          <bgColor rgb="FF9BC2E6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1039,6 +1536,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB2CF70C-C2E0-4923-967F-E2CB5633FE2F}" name="Tableau1" displayName="Tableau1" ref="A112:L146" totalsRowShown="0" tableBorderDxfId="12">
+  <autoFilter ref="A112:L146" xr:uid="{74CE8FF5-0809-41A9-A888-3822A57DF07F}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{74896ED9-56DB-48E8-969A-A2192FEC9341}" name="Order" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{1D76CB1C-FBDC-4AF5-B780-42DFF9410A1C}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{ACFD7474-C6F4-4E67-B814-9CD438DD0A9F}" name="Mode Start" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{A6D964A7-24B9-4523-A078-1F6FE1732C62}" name="Trigger" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{482AB9F0-C37F-4C9E-A66E-97DECB219FE4}" name="Weather" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{315AE578-AF89-4D62-8871-ED5FC6CCD312}" name="Road" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{970D5CF1-9381-4F01-A4AB-5A1A12C86329}" name="Traffic" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{CE9F20B2-489B-488D-BD40-DFF63DF51A80}" name="Vehicle" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{EB7591B6-6887-46E8-82E0-8FF0AE2EEEC1}" name="Human" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{23F12F3C-DC47-4316-B282-CEA1F9CDA986}" name="Mode (End)"/>
+    <tableColumn id="10" xr3:uid="{547B9250-5BCF-479B-9A44-42AD9B31EF0C}" name="Objective" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{4BCF60A5-7D56-46E1-ABD8-FBD62BE36937}" name="Comments" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1242,16 +1760,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB152"/>
+  <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" topLeftCell="C106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="1" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
@@ -1264,28 +1781,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="89" t="s">
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="82" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="80" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A2" s="88"/>
+      <c r="A2" s="81"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1301,11 +1818,11 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="88"/>
+      <c r="G2" s="81"/>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="88"/>
+      <c r="I2" s="81"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" hidden="1" customHeight="1">
       <c r="A3" s="3"/>
@@ -5283,19 +5800,18 @@
     </row>
     <row r="107" spans="1:28" ht="15">
       <c r="A107" s="48"/>
-      <c r="B107" s="49" t="s">
+      <c r="C107" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C107" s="50" t="s">
+      <c r="D107" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D107" s="66" t="s">
+      <c r="E107" s="65" t="s">
         <v>175</v>
       </c>
-      <c r="E107" s="51" t="s">
+      <c r="F107" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F107" s="47"/>
       <c r="G107" s="52"/>
       <c r="H107" s="52"/>
       <c r="I107" s="53"/>
@@ -5320,1170 +5836,1296 @@
       <c r="AB107" s="53"/>
     </row>
     <row r="108" spans="1:28" ht="15">
-      <c r="A108" s="93"/>
-      <c r="B108" s="93" t="s">
+      <c r="A108" s="86"/>
+      <c r="C108" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="C108" s="94"/>
-      <c r="D108" s="94"/>
-      <c r="E108" s="94"/>
-      <c r="F108" s="94"/>
-      <c r="G108" s="93"/>
-      <c r="H108" s="95"/>
+      <c r="D108" s="86"/>
+      <c r="E108" s="86"/>
+      <c r="F108" s="86"/>
+      <c r="G108" s="86"/>
+      <c r="H108" s="88"/>
     </row>
     <row r="109" spans="1:28" ht="15">
-      <c r="A109" s="94"/>
-      <c r="B109" s="93" t="s">
+      <c r="A109" s="87"/>
+      <c r="C109" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="C109" s="94"/>
-      <c r="D109" s="94"/>
-      <c r="E109" s="55"/>
-      <c r="F109" s="55"/>
-      <c r="G109" s="94"/>
-      <c r="H109" s="94"/>
-    </row>
-    <row r="110" spans="1:28" ht="15">
-      <c r="A110" s="54"/>
-      <c r="B110" s="55"/>
-      <c r="C110" s="55"/>
-      <c r="D110" s="55"/>
-      <c r="E110" s="55"/>
-      <c r="F110" s="55"/>
-      <c r="G110" s="55"/>
-      <c r="H110" s="56"/>
+      <c r="D109" s="86"/>
+      <c r="E109" s="86"/>
+      <c r="F109" s="86"/>
+      <c r="G109" s="87"/>
+      <c r="H109" s="87"/>
+    </row>
+    <row r="110" spans="1:28" s="78" customFormat="1" ht="15">
+      <c r="B110" s="77"/>
+      <c r="E110" s="77"/>
+      <c r="F110" s="77"/>
     </row>
     <row r="111" spans="1:28" ht="15">
-      <c r="A111" s="89" t="s">
+      <c r="A111" s="54"/>
+      <c r="C111" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" s="106"/>
+      <c r="E111" s="106"/>
+      <c r="F111" s="106"/>
+      <c r="G111" s="106"/>
+      <c r="H111" s="106"/>
+      <c r="I111" s="106"/>
+      <c r="J111" s="106"/>
+    </row>
+    <row r="112" spans="1:28" ht="15">
+      <c r="A112" s="89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B111" s="90" t="s">
+      <c r="C112" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G112" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="H112" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="I112" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K112" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="L112" s="91" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A113" s="57">
         <v>1</v>
       </c>
-      <c r="C111" s="91"/>
-      <c r="D111" s="91"/>
-      <c r="E111" s="91"/>
-      <c r="F111" s="91"/>
-      <c r="G111" s="91"/>
-      <c r="H111" s="91"/>
-      <c r="I111" s="57"/>
-      <c r="J111" s="96" t="s">
+      <c r="B113" s="57">
+        <v>1</v>
+      </c>
+      <c r="C113" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="E113" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="F113" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="G113" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H113" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="I113" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="J113" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K113" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="L113" s="92"/>
+    </row>
+    <row r="114" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A114" s="57">
+        <f>A113+1</f>
         <v>2</v>
       </c>
-      <c r="K111" s="87" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="112" spans="1:28" ht="15">
-      <c r="A112" s="88"/>
-      <c r="B112" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F112" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="G112" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="H112" s="58" t="s">
+      <c r="B114" s="57">
+        <v>2</v>
+      </c>
+      <c r="C114" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E114" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="F114" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G114" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H114" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="I114" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="J114" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K114" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="L114" s="92"/>
+    </row>
+    <row r="115" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A115" s="57">
+        <f t="shared" ref="A115:A146" si="0">A114+1</f>
+        <v>3</v>
+      </c>
+      <c r="B115" s="57">
+        <v>3</v>
+      </c>
+      <c r="C115" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E115" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F115" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G115" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H115" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I115" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="J115" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="K115" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="L115" s="92" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A116" s="57">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B116" s="57">
+        <v>4</v>
+      </c>
+      <c r="C116" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E116" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F116" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G116" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H116" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I116" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="J116" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="K116" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="L116" s="92" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A117" s="57">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B117" s="57">
+        <v>5</v>
+      </c>
+      <c r="C117" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E117" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F117" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G117" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H117" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I117" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="J117" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K117" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="L117" s="92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A118" s="57">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B118" s="59">
+        <v>6</v>
+      </c>
+      <c r="C118" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="E118" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="F118" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G118" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H118" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I118" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="J118" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K118" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="L118" s="92" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" s="75" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A119" s="57">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B119" s="57">
+        <v>7</v>
+      </c>
+      <c r="C119" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E119" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F119" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G119" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H119" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I119" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="J119" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K119" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="L119" s="92"/>
+    </row>
+    <row r="120" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A120" s="74">
         <v>8</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="B120" s="74"/>
+      <c r="C120" s="74"/>
+      <c r="D120" s="74"/>
+      <c r="E120" s="74"/>
+      <c r="F120" s="74"/>
+      <c r="G120" s="74"/>
+      <c r="H120" s="74"/>
+      <c r="I120" s="74"/>
+      <c r="J120" s="74"/>
+      <c r="K120" s="74"/>
+      <c r="L120" s="93"/>
+    </row>
+    <row r="121" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A121" s="57">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J112" s="88"/>
-      <c r="K112" s="88"/>
-    </row>
-    <row r="113" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A113" s="69">
-        <v>1</v>
-      </c>
-      <c r="B113" s="70" t="s">
+      <c r="B121" s="57">
+        <v>8</v>
+      </c>
+      <c r="C121" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D121" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="E121" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="F121" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="G121" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H121" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I121" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="J121" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K121" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="L121" s="92"/>
+    </row>
+    <row r="122" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A122" s="57">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B122" s="57">
+        <v>9</v>
+      </c>
+      <c r="C122" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D122" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="E122" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="F122" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="G122" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H122" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="I122" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="J122" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K122" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="L122" s="92" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A123" s="57">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C113" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="D113" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="E113" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="F113" s="59" t="s">
+      <c r="B123" s="57">
+        <v>10</v>
+      </c>
+      <c r="C123" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D123" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="E123" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="F123" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G123" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="H123" s="67" t="s">
+        <v>108</v>
+      </c>
+      <c r="I123" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="J123" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K123" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="L123" s="92"/>
+    </row>
+    <row r="124" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A124" s="57">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B124" s="57">
+        <v>11</v>
+      </c>
+      <c r="C124" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D124" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="E124" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F124" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G124" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="G113" s="59" t="s">
+      <c r="H124" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="H113" s="59" t="s">
+      <c r="I124" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="J124" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K124" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="L124" s="92"/>
+    </row>
+    <row r="125" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A125" s="57">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B125" s="57">
+        <v>12</v>
+      </c>
+      <c r="C125" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D125" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="E125" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F125" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G125" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H125" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I125" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="J125" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K125" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="L125" s="92"/>
+    </row>
+    <row r="126" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A126" s="57">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B126" s="57">
+        <v>13</v>
+      </c>
+      <c r="C126" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D126" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E126" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F126" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G126" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H126" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I126" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="J126" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K126" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="L126" s="92"/>
+    </row>
+    <row r="127" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A127" s="57">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B127" s="57">
+        <v>14</v>
+      </c>
+      <c r="C127" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D127" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E127" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F127" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G127" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H127" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I127" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="I113" s="59" t="s">
+      <c r="J127" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K127" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="L127" s="92"/>
+    </row>
+    <row r="128" spans="1:12" s="75" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A128" s="57">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B128" s="57">
         <v>15</v>
       </c>
-      <c r="J113" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="K113" s="71"/>
-    </row>
-    <row r="114" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A114" s="69">
-        <v>2</v>
-      </c>
-      <c r="B114" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C114" s="61" t="s">
+      <c r="C128" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D128" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E128" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="F128" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G128" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H128" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I128" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="J128" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K128" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="L128" s="92"/>
+    </row>
+    <row r="129" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A129" s="74">
+        <v>17</v>
+      </c>
+      <c r="B129" s="74"/>
+      <c r="C129" s="74"/>
+      <c r="D129" s="74"/>
+      <c r="E129" s="74"/>
+      <c r="F129" s="74"/>
+      <c r="G129" s="74"/>
+      <c r="H129" s="74"/>
+      <c r="I129" s="74"/>
+      <c r="J129" s="74"/>
+      <c r="K129" s="74"/>
+      <c r="L129" s="93"/>
+    </row>
+    <row r="130" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A130" s="57">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B130" s="57">
+        <v>16</v>
+      </c>
+      <c r="C130" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D130" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E130" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="F130" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G130" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H130" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I130" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="J130" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K130" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="L130" s="92"/>
+    </row>
+    <row r="131" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A131" s="57">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B131" s="57">
+        <v>17</v>
+      </c>
+      <c r="C131" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D131" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="D114" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="E114" s="60" t="s">
+      <c r="E131" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F131" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="F114" s="60" t="s">
+      <c r="G131" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="G114" s="61" t="s">
+      <c r="H131" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="H114" s="59" t="s">
+      <c r="I131" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="J131" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="K131" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="L131" s="92" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A132" s="57">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B132" s="57">
+        <v>18</v>
+      </c>
+      <c r="C132" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D132" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E132" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F132" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G132" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H132" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I132" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="J132" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K132" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="L132" s="92" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A133" s="57">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B133" s="57">
+        <v>19</v>
+      </c>
+      <c r="C133" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D133" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E133" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="F133" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G133" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H133" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I133" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="J133" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K133" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="L133" s="92" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A134" s="57">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B134" s="57">
+        <v>20</v>
+      </c>
+      <c r="C134" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D134" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="E134" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F134" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G134" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H134" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="I134" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="J134" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K134" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="L134" s="92"/>
+    </row>
+    <row r="135" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A135" s="57">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B135" s="90">
+        <v>21</v>
+      </c>
+      <c r="C135" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D135" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="E135" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F135" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G135" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H135" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I135" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="I114" s="59" t="s">
+      <c r="J135" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K135" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="L135" s="94"/>
+    </row>
+    <row r="136" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A136" s="57">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B136" s="90">
+        <v>22</v>
+      </c>
+      <c r="C136" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D136" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="E136" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F136" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G136" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H136" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I136" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="J136" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K136" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="L136" s="94"/>
+    </row>
+    <row r="137" spans="1:12" s="75" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A137" s="57">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B137" s="90">
+        <v>23</v>
+      </c>
+      <c r="C137" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D137" s="60" t="s">
+        <v>161</v>
+      </c>
+      <c r="E137" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F137" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G137" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H137" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I137" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="J137" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="K137" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="L137" s="94"/>
+    </row>
+    <row r="138" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A138" s="76">
+        <v>26</v>
+      </c>
+      <c r="B138" s="76"/>
+      <c r="C138" s="76"/>
+      <c r="D138" s="76"/>
+      <c r="E138" s="76"/>
+      <c r="F138" s="76"/>
+      <c r="G138" s="76"/>
+      <c r="H138" s="76"/>
+      <c r="I138" s="76"/>
+      <c r="J138" s="76"/>
+      <c r="K138" s="76"/>
+      <c r="L138" s="95"/>
+    </row>
+    <row r="139" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A139" s="57">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B139" s="90">
+        <v>24</v>
+      </c>
+      <c r="C139" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D139" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="E139" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F139" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="G139" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H139" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I139" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="J139" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="J114" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="K114" s="71"/>
-    </row>
-    <row r="115" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A115" s="69">
-        <v>3</v>
-      </c>
-      <c r="B115" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C115" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="D115" s="60" t="s">
+      <c r="K139" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L139" s="94"/>
+    </row>
+    <row r="140" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A140" s="57">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B140" s="90">
+        <v>25</v>
+      </c>
+      <c r="C140" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D140" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E140" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="E115" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="F115" s="59" t="s">
+      <c r="F140" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="G140" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="G115" s="60" t="s">
+      <c r="H140" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="I140" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="J140" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="K140" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L140" s="94"/>
+    </row>
+    <row r="141" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A141" s="57">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B141" s="90">
+        <v>26</v>
+      </c>
+      <c r="C141" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D141" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="E141" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F141" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G141" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="H141" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="H115" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="I115" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="J115" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="K115" s="71" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A116" s="69">
-        <v>4</v>
-      </c>
-      <c r="B116" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C116" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D116" s="60" t="s">
+      <c r="I141" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="J141" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K141" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="L141" s="94" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A142" s="57">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B142" s="90">
+        <v>27</v>
+      </c>
+      <c r="C142" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D142" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="E142" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="E116" s="60" t="s">
+      <c r="F142" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="F116" s="60" t="s">
+      <c r="G142" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="H142" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I142" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="J142" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K142" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="L142" s="94"/>
+    </row>
+    <row r="143" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A143" s="57">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B143" s="90">
+        <v>28</v>
+      </c>
+      <c r="C143" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D143" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="E143" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F143" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G143" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="G116" s="60" t="s">
+      <c r="H143" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="H116" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="I116" s="60" t="s">
+      <c r="I143" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="J143" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="K143" s="72" t="s">
+        <v>173</v>
+      </c>
+      <c r="L143" s="94"/>
+    </row>
+    <row r="144" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A144" s="57">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B144" s="90">
+        <v>29</v>
+      </c>
+      <c r="C144" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D144" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E144" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F144" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G144" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H144" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I144" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="J144" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="K144" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="L144" s="94"/>
+    </row>
+    <row r="145" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A145" s="57">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B145" s="90">
+        <v>30</v>
+      </c>
+      <c r="C145" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D145" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="E145" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F145" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G145" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H145" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="I145" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="J145" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="J116" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="K116" s="71" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A117" s="69">
-        <v>5</v>
-      </c>
-      <c r="B117" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C117" s="61" t="s">
-        <v>122</v>
-      </c>
-      <c r="D117" s="60" t="s">
+      <c r="K145" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="L145" s="94"/>
+    </row>
+    <row r="146" spans="1:12" ht="30">
+      <c r="A146" s="57">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B146" s="97">
+        <v>31</v>
+      </c>
+      <c r="C146" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="D146" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="E146" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="E117" s="60" t="s">
+      <c r="F146" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="F117" s="60" t="s">
+      <c r="G146" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="G117" s="60" t="s">
+      <c r="H146" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="H117" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="I117" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="J117" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="K117" s="71" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A118" s="73">
-        <v>6</v>
-      </c>
-      <c r="B118" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" s="61" t="s">
-        <v>126</v>
-      </c>
-      <c r="D118" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="E118" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F118" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G118" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H118" s="61" t="s">
-        <v>128</v>
-      </c>
-      <c r="I118" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J118" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="K118" s="71" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A119" s="69">
-        <v>7</v>
-      </c>
-      <c r="B119" s="70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D119" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E119" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F119" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G119" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H119" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="I119" s="59" t="s">
+      <c r="I146" s="102" t="s">
+        <v>162</v>
+      </c>
+      <c r="J146" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="J119" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="K119" s="71"/>
-    </row>
-    <row r="120" spans="1:11" s="83" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A120" s="80"/>
-      <c r="B120" s="81"/>
-      <c r="C120" s="81"/>
-      <c r="D120" s="81"/>
-      <c r="E120" s="81"/>
-      <c r="F120" s="81"/>
-      <c r="G120" s="81"/>
-      <c r="H120" s="81"/>
-      <c r="I120" s="81"/>
-      <c r="J120" s="81"/>
-      <c r="K120" s="82"/>
-    </row>
-    <row r="121" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A121" s="69">
-        <v>8</v>
-      </c>
-      <c r="B121" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C121" s="61" t="s">
-        <v>132</v>
-      </c>
-      <c r="D121" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="E121" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="F121" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G121" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H121" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="I121" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="J121" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="K121" s="71"/>
-    </row>
-    <row r="122" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A122" s="69">
-        <v>9</v>
-      </c>
-      <c r="B122" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C122" s="61" t="s">
-        <v>135</v>
-      </c>
-      <c r="D122" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="E122" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="F122" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G122" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="H122" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="I122" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="J122" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="K122" s="71" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A123" s="69">
-        <v>10</v>
-      </c>
-      <c r="B123" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C123" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="D123" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="E123" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F123" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="G123" s="68" t="s">
-        <v>108</v>
-      </c>
-      <c r="H123" s="61" t="s">
-        <v>139</v>
-      </c>
-      <c r="I123" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="J123" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="K123" s="71"/>
-    </row>
-    <row r="124" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A124" s="69">
-        <v>11</v>
-      </c>
-      <c r="B124" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C124" s="61" t="s">
-        <v>141</v>
-      </c>
-      <c r="D124" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E124" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="F124" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G124" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H124" s="61" t="s">
-        <v>142</v>
-      </c>
-      <c r="I124" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="J124" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="K124" s="71"/>
-    </row>
-    <row r="125" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A125" s="69">
-        <v>12</v>
-      </c>
-      <c r="B125" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C125" s="61" t="s">
-        <v>141</v>
-      </c>
-      <c r="D125" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E125" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F125" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G125" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H125" s="61" t="s">
-        <v>142</v>
-      </c>
-      <c r="I125" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J125" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="K125" s="71"/>
-    </row>
-    <row r="126" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A126" s="69">
-        <v>13</v>
-      </c>
-      <c r="B126" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C126" s="61" t="s">
-        <v>122</v>
-      </c>
-      <c r="D126" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E126" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F126" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G126" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H126" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="I126" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="J126" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="K126" s="71"/>
-    </row>
-    <row r="127" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A127" s="69">
-        <v>14</v>
-      </c>
-      <c r="B127" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C127" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D127" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E127" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F127" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G127" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H127" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="I127" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J127" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="K127" s="71"/>
-    </row>
-    <row r="128" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A128" s="69">
-        <v>15</v>
-      </c>
-      <c r="B128" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C128" s="61" t="s">
-        <v>145</v>
-      </c>
-      <c r="D128" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="E128" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F128" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G128" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H128" s="61" t="s">
-        <v>139</v>
-      </c>
-      <c r="I128" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J128" s="59" t="s">
-        <v>146</v>
-      </c>
-      <c r="K128" s="71"/>
-    </row>
-    <row r="129" spans="1:11" s="83" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A129" s="80"/>
-      <c r="B129" s="81"/>
-      <c r="C129" s="81"/>
-      <c r="D129" s="81"/>
-      <c r="E129" s="81"/>
-      <c r="F129" s="81"/>
-      <c r="G129" s="81"/>
-      <c r="H129" s="81"/>
-      <c r="I129" s="81"/>
-      <c r="J129" s="81"/>
-      <c r="K129" s="82"/>
-    </row>
-    <row r="130" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A130" s="69">
-        <v>17</v>
-      </c>
-      <c r="B130" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C130" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="D130" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="E130" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F130" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G130" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H130" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="I130" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J130" s="59" t="s">
-        <v>149</v>
-      </c>
-      <c r="K130" s="71"/>
-    </row>
-    <row r="131" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A131" s="69">
-        <v>18</v>
-      </c>
-      <c r="B131" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C131" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="D131" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E131" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F131" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G131" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="H131" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="I131" s="59" t="s">
-        <v>114</v>
-      </c>
-      <c r="J131" s="59" t="s">
-        <v>65</v>
-      </c>
-      <c r="K131" s="71" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A132" s="69">
-        <v>19</v>
-      </c>
-      <c r="B132" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C132" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="D132" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E132" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F132" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G132" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H132" s="61" t="s">
-        <v>152</v>
-      </c>
-      <c r="I132" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J132" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="K132" s="71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A133" s="69">
-        <v>20</v>
-      </c>
-      <c r="B133" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C133" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D133" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="E133" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F133" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G133" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="H133" s="61" t="s">
-        <v>154</v>
-      </c>
-      <c r="I133" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="J133" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="K133" s="71" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A134" s="69">
-        <v>21</v>
-      </c>
-      <c r="B134" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C134" s="61" t="s">
-        <v>156</v>
-      </c>
-      <c r="D134" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E134" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="F134" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G134" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="H134" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="I134" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="J134" s="74" t="s">
-        <v>124</v>
-      </c>
-      <c r="K134" s="71"/>
-    </row>
-    <row r="135" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A135" s="75">
-        <v>22</v>
-      </c>
-      <c r="B135" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="C135" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="D135" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E135" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F135" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G135" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H135" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="I135" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J135" s="74" t="s">
-        <v>158</v>
-      </c>
-      <c r="K135" s="77"/>
-    </row>
-    <row r="136" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A136" s="75">
-        <v>23</v>
-      </c>
-      <c r="B136" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="C136" s="61" t="s">
-        <v>126</v>
-      </c>
-      <c r="D136" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E136" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F136" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G136" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H136" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="I136" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J136" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="K136" s="77"/>
-    </row>
-    <row r="137" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A137" s="75">
-        <v>24</v>
-      </c>
-      <c r="B137" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="C137" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="D137" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E137" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F137" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G137" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H137" s="63" t="s">
-        <v>162</v>
-      </c>
-      <c r="I137" s="74" t="s">
-        <v>114</v>
-      </c>
-      <c r="J137" s="74" t="s">
-        <v>163</v>
-      </c>
-      <c r="K137" s="77"/>
-    </row>
-    <row r="138" spans="1:11" s="83" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A138" s="84"/>
-      <c r="B138" s="85"/>
-      <c r="C138" s="85"/>
-      <c r="D138" s="85"/>
-      <c r="E138" s="85"/>
-      <c r="F138" s="85"/>
-      <c r="G138" s="85"/>
-      <c r="H138" s="85"/>
-      <c r="I138" s="85"/>
-      <c r="J138" s="85"/>
-      <c r="K138" s="86"/>
-    </row>
-    <row r="139" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A139" s="75">
-        <v>25</v>
-      </c>
-      <c r="B139" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C139" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="D139" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E139" s="63" t="s">
-        <v>164</v>
-      </c>
-      <c r="F139" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G139" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H139" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="I139" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="J139" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="K139" s="77"/>
-    </row>
-    <row r="140" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A140" s="75">
-        <v>26</v>
-      </c>
-      <c r="B140" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C140" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="D140" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E140" s="67" t="s">
-        <v>164</v>
-      </c>
-      <c r="F140" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="G140" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="H140" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="I140" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="J140" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="K140" s="77"/>
-    </row>
-    <row r="141" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A141" s="75">
-        <v>27</v>
-      </c>
-      <c r="B141" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C141" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="D141" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E141" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F141" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="G141" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H141" s="61" t="s">
-        <v>168</v>
-      </c>
-      <c r="I141" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J141" s="62" t="s">
-        <v>169</v>
-      </c>
-      <c r="K141" s="77" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A142" s="75">
-        <v>28</v>
-      </c>
-      <c r="B142" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C142" s="61" t="s">
-        <v>141</v>
-      </c>
-      <c r="D142" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E142" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F142" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="G142" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H142" s="61" t="s">
-        <v>142</v>
-      </c>
-      <c r="I142" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J142" s="78" t="s">
-        <v>171</v>
-      </c>
-      <c r="K142" s="77"/>
-    </row>
-    <row r="143" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A143" s="75">
-        <v>29</v>
-      </c>
-      <c r="B143" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C143" s="61" t="s">
-        <v>122</v>
-      </c>
-      <c r="D143" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E143" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F143" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G143" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H143" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="I143" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="J143" s="78" t="s">
-        <v>173</v>
-      </c>
-      <c r="K143" s="77"/>
-    </row>
-    <row r="144" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A144" s="75">
-        <v>30</v>
-      </c>
-      <c r="B144" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C144" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D144" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E144" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F144" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G144" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H144" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="I144" s="79" t="s">
-        <v>15</v>
-      </c>
-      <c r="J144" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="K144" s="77"/>
-    </row>
-    <row r="145" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A145" s="75">
-        <v>31</v>
-      </c>
-      <c r="B145" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C145" s="61" t="s">
-        <v>126</v>
-      </c>
-      <c r="D145" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E145" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F145" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G145" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H145" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="I145" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="J145" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="K145" s="77"/>
-    </row>
-    <row r="146" spans="1:11" s="72" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A146" s="75">
-        <v>32</v>
-      </c>
-      <c r="B146" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C146" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="D146" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="E146" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="F146" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="G146" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="H146" s="63" t="s">
-        <v>162</v>
-      </c>
-      <c r="I146" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="J146" s="62" t="s">
+      <c r="K146" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="K146" s="77"/>
-    </row>
-    <row r="147" spans="1:11" ht="15">
+      <c r="L146" s="104"/>
+    </row>
+    <row r="147" spans="1:12" ht="15">
       <c r="A147" s="54"/>
       <c r="B147" s="55"/>
       <c r="C147" s="55"/>
@@ -6493,7 +7135,7 @@
       <c r="G147" s="55"/>
       <c r="H147" s="64"/>
     </row>
-    <row r="148" spans="1:11" ht="15">
+    <row r="148" spans="1:12" ht="15">
       <c r="A148" s="54"/>
       <c r="B148" s="55"/>
       <c r="C148" s="55"/>
@@ -6501,19 +7143,19 @@
       <c r="E148" s="55"/>
       <c r="F148" s="55"/>
       <c r="G148" s="55"/>
-      <c r="H148" s="65"/>
-    </row>
-    <row r="149" spans="1:11" ht="15">
+      <c r="H148" s="63"/>
+    </row>
+    <row r="149" spans="1:12" ht="15">
       <c r="A149" s="54"/>
-      <c r="B149" s="55"/>
+      <c r="B149" s="56"/>
       <c r="C149" s="55"/>
       <c r="D149" s="55"/>
       <c r="E149" s="55"/>
       <c r="F149" s="55"/>
       <c r="G149" s="55"/>
-      <c r="H149" s="64"/>
-    </row>
-    <row r="150" spans="1:11" ht="15">
+      <c r="H149" s="63"/>
+    </row>
+    <row r="150" spans="1:12" ht="15">
       <c r="A150" s="54"/>
       <c r="B150" s="56"/>
       <c r="C150" s="55"/>
@@ -6521,9 +7163,9 @@
       <c r="E150" s="55"/>
       <c r="F150" s="55"/>
       <c r="G150" s="55"/>
-      <c r="H150" s="64"/>
-    </row>
-    <row r="151" spans="1:11" ht="15">
+      <c r="H150" s="63"/>
+    </row>
+    <row r="151" spans="1:12" ht="15">
       <c r="A151" s="54"/>
       <c r="B151" s="56"/>
       <c r="C151" s="55"/>
@@ -6531,21 +7173,11 @@
       <c r="E151" s="55"/>
       <c r="F151" s="55"/>
       <c r="G151" s="55"/>
-      <c r="H151" s="64"/>
-    </row>
-    <row r="152" spans="1:11" ht="15">
-      <c r="A152" s="54"/>
-      <c r="B152" s="56"/>
-      <c r="C152" s="55"/>
-      <c r="D152" s="55"/>
-      <c r="E152" s="55"/>
-      <c r="F152" s="55"/>
-      <c r="G152" s="55"/>
-      <c r="H152" s="64"/>
+      <c r="H151" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="K111:K112"/>
+  <mergeCells count="10">
+    <mergeCell ref="C109:F109"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:G2"/>
@@ -6553,17 +7185,17 @@
     <mergeCell ref="A108:A109"/>
     <mergeCell ref="G108:G109"/>
     <mergeCell ref="H108:H109"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="B111:H111"/>
-    <mergeCell ref="J111:J112"/>
+    <mergeCell ref="C111:J111"/>
+    <mergeCell ref="C108:F108"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:I104 B130:B146">
+  <conditionalFormatting sqref="A1:I104 C130:C146">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout conversions variables en CCSL + Modulation operateurs en TextScade
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8048C047-CE91-423B-8BB5-82CB8F08B1D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1555C257-378B-4832-819D-493D4AD5BD06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -818,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1009,12 +1009,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1031,130 +1025,102 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1510,6 +1476,44 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1525,6 +1529,14 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1539,21 +1551,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB2CF70C-C2E0-4923-967F-E2CB5633FE2F}" name="Tableau1" displayName="Tableau1" ref="A112:L146" totalsRowShown="0" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB2CF70C-C2E0-4923-967F-E2CB5633FE2F}" name="Tableau1" displayName="Tableau1" ref="A112:L146" totalsRowShown="0" tableBorderDxfId="11">
   <autoFilter ref="A112:L146" xr:uid="{74CE8FF5-0809-41A9-A888-3822A57DF07F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A113:L146">
+    <sortCondition ref="A112:A146"/>
+  </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{74896ED9-56DB-48E8-969A-A2192FEC9341}" name="Order" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{1D76CB1C-FBDC-4AF5-B780-42DFF9410A1C}" name="ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{ACFD7474-C6F4-4E67-B814-9CD438DD0A9F}" name="Mode Start" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A6D964A7-24B9-4523-A078-1F6FE1732C62}" name="Trigger" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{482AB9F0-C37F-4C9E-A66E-97DECB219FE4}" name="Weather" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{315AE578-AF89-4D62-8871-ED5FC6CCD312}" name="Road" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{970D5CF1-9381-4F01-A4AB-5A1A12C86329}" name="Traffic" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{CE9F20B2-489B-488D-BD40-DFF63DF51A80}" name="Vehicle" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{EB7591B6-6887-46E8-82E0-8FF0AE2EEEC1}" name="Human" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{74896ED9-56DB-48E8-969A-A2192FEC9341}" name="Order" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{1D76CB1C-FBDC-4AF5-B780-42DFF9410A1C}" name="ID" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{ACFD7474-C6F4-4E67-B814-9CD438DD0A9F}" name="Mode Start" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{A6D964A7-24B9-4523-A078-1F6FE1732C62}" name="Trigger" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{482AB9F0-C37F-4C9E-A66E-97DECB219FE4}" name="Weather" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{315AE578-AF89-4D62-8871-ED5FC6CCD312}" name="Road" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{970D5CF1-9381-4F01-A4AB-5A1A12C86329}" name="Traffic" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{CE9F20B2-489B-488D-BD40-DFF63DF51A80}" name="Vehicle" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{EB7591B6-6887-46E8-82E0-8FF0AE2EEEC1}" name="Human" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{23F12F3C-DC47-4316-B282-CEA1F9CDA986}" name="Mode (End)"/>
-    <tableColumn id="10" xr3:uid="{547B9250-5BCF-479B-9A44-42AD9B31EF0C}" name="Objective" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{4BCF60A5-7D56-46E1-ABD8-FBD62BE36937}" name="Comments" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{547B9250-5BCF-479B-9A44-42AD9B31EF0C}" name="Objective" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{4BCF60A5-7D56-46E1-ABD8-FBD62BE36937}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1762,8 +1777,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1781,28 +1796,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="82" t="s">
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="95" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="I1" s="100" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A2" s="81"/>
+      <c r="A2" s="96"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1818,11 +1833,11 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="81"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="81"/>
+      <c r="I2" s="96"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" hidden="1" customHeight="1">
       <c r="A3" s="3"/>
@@ -5836,50 +5851,50 @@
       <c r="AB107" s="53"/>
     </row>
     <row r="108" spans="1:28" ht="15">
-      <c r="A108" s="86"/>
-      <c r="C108" s="86" t="s">
+      <c r="A108" s="94"/>
+      <c r="C108" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="D108" s="86"/>
-      <c r="E108" s="86"/>
-      <c r="F108" s="86"/>
-      <c r="G108" s="86"/>
-      <c r="H108" s="88"/>
+      <c r="D108" s="94"/>
+      <c r="E108" s="94"/>
+      <c r="F108" s="94"/>
+      <c r="G108" s="94"/>
+      <c r="H108" s="102"/>
     </row>
     <row r="109" spans="1:28" ht="15">
-      <c r="A109" s="87"/>
-      <c r="C109" s="86" t="s">
+      <c r="A109" s="101"/>
+      <c r="C109" s="94" t="s">
         <v>92</v>
       </c>
-      <c r="D109" s="86"/>
-      <c r="E109" s="86"/>
-      <c r="F109" s="86"/>
-      <c r="G109" s="87"/>
-      <c r="H109" s="87"/>
-    </row>
-    <row r="110" spans="1:28" s="78" customFormat="1" ht="15">
-      <c r="B110" s="77"/>
-      <c r="E110" s="77"/>
-      <c r="F110" s="77"/>
+      <c r="D109" s="94"/>
+      <c r="E109" s="94"/>
+      <c r="F109" s="94"/>
+      <c r="G109" s="101"/>
+      <c r="H109" s="101"/>
+    </row>
+    <row r="110" spans="1:28" s="76" customFormat="1" ht="15">
+      <c r="B110" s="75"/>
+      <c r="E110" s="75"/>
+      <c r="F110" s="75"/>
     </row>
     <row r="111" spans="1:28" ht="15">
       <c r="A111" s="54"/>
-      <c r="C111" s="105" t="s">
+      <c r="C111" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="D111" s="106"/>
-      <c r="E111" s="106"/>
-      <c r="F111" s="106"/>
-      <c r="G111" s="106"/>
-      <c r="H111" s="106"/>
-      <c r="I111" s="106"/>
-      <c r="J111" s="106"/>
+      <c r="D111" s="104"/>
+      <c r="E111" s="104"/>
+      <c r="F111" s="104"/>
+      <c r="G111" s="104"/>
+      <c r="H111" s="104"/>
+      <c r="I111" s="104"/>
+      <c r="J111" s="104"/>
     </row>
     <row r="112" spans="1:28" ht="15">
-      <c r="A112" s="89" t="s">
+      <c r="A112" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="B112" s="96" t="s">
+      <c r="B112" s="85" t="s">
         <v>0</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -5906,10 +5921,10 @@
       <c r="J112" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K112" s="79" t="s">
+      <c r="K112" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="L112" s="91" t="s">
+      <c r="L112" s="80" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5947,7 +5962,7 @@
       <c r="K113" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="L113" s="92"/>
+      <c r="L113" s="81"/>
     </row>
     <row r="114" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A114" s="57">
@@ -5984,11 +5999,11 @@
       <c r="K114" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="L114" s="92"/>
+      <c r="L114" s="81"/>
     </row>
     <row r="115" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A115" s="57">
-        <f t="shared" ref="A115:A146" si="0">A114+1</f>
+        <f>A114+1</f>
         <v>3</v>
       </c>
       <c r="B115" s="57">
@@ -6021,13 +6036,13 @@
       <c r="K115" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="L115" s="92" t="s">
+      <c r="L115" s="81" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A116" s="57">
-        <f t="shared" si="0"/>
+        <f>A115+1</f>
         <v>4</v>
       </c>
       <c r="B116" s="57">
@@ -6060,13 +6075,13 @@
       <c r="K116" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="L116" s="92" t="s">
+      <c r="L116" s="81" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A117" s="57">
-        <f t="shared" si="0"/>
+        <f>A116+1</f>
         <v>5</v>
       </c>
       <c r="B117" s="57">
@@ -6099,13 +6114,13 @@
       <c r="K117" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="L117" s="92" t="s">
+      <c r="L117" s="81" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="118" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A118" s="57">
-        <f t="shared" si="0"/>
+        <f>A117+1</f>
         <v>6</v>
       </c>
       <c r="B118" s="59">
@@ -6138,13 +6153,13 @@
       <c r="K118" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="L118" s="92" t="s">
+      <c r="L118" s="81" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="1:12" s="75" customFormat="1" ht="29.45" customHeight="1">
+    <row r="119" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A119" s="57">
-        <f t="shared" si="0"/>
+        <f>A118+1</f>
         <v>7</v>
       </c>
       <c r="B119" s="57">
@@ -6177,65 +6192,65 @@
       <c r="K119" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="L119" s="92"/>
+      <c r="L119" s="81"/>
     </row>
     <row r="120" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A120" s="74">
+      <c r="A120" s="57">
+        <f>A119+1</f>
         <v>8</v>
       </c>
-      <c r="B120" s="74"/>
-      <c r="C120" s="74"/>
-      <c r="D120" s="74"/>
-      <c r="E120" s="74"/>
-      <c r="F120" s="74"/>
-      <c r="G120" s="74"/>
-      <c r="H120" s="74"/>
-      <c r="I120" s="74"/>
-      <c r="J120" s="74"/>
-      <c r="K120" s="74"/>
-      <c r="L120" s="93"/>
+      <c r="B120" s="57">
+        <v>8</v>
+      </c>
+      <c r="C120" s="68" t="s">
+        <v>174</v>
+      </c>
+      <c r="D120" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="E120" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="F120" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="G120" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H120" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I120" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="J120" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="K120" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="L120" s="81"/>
     </row>
     <row r="121" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A121" s="57">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B121" s="57">
+      <c r="A121" s="72">
         <v>8</v>
       </c>
-      <c r="C121" s="68" t="s">
-        <v>174</v>
-      </c>
-      <c r="D121" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="E121" s="60" t="s">
-        <v>127</v>
-      </c>
-      <c r="F121" s="59" t="s">
-        <v>133</v>
-      </c>
-      <c r="G121" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="H121" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="I121" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="J121" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="K121" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="L121" s="92"/>
+      <c r="B121" s="72"/>
+      <c r="C121" s="72"/>
+      <c r="D121" s="72"/>
+      <c r="E121" s="72"/>
+      <c r="F121" s="72"/>
+      <c r="G121" s="72"/>
+      <c r="H121" s="72"/>
+      <c r="I121" s="72"/>
+      <c r="J121" s="72"/>
+      <c r="K121" s="72"/>
+      <c r="L121" s="82"/>
     </row>
     <row r="122" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A122" s="57">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>A121+1</f>
+        <v>9</v>
       </c>
       <c r="B122" s="57">
         <v>9</v>
@@ -6267,38 +6282,38 @@
       <c r="K122" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="L122" s="92" t="s">
+      <c r="L122" s="81" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A123" s="57">
-        <f t="shared" si="0"/>
+        <f>A122+1</f>
+        <v>10</v>
+      </c>
+      <c r="B123" s="57">
         <v>11</v>
-      </c>
-      <c r="B123" s="57">
-        <v>10</v>
       </c>
       <c r="C123" s="68" t="s">
         <v>174</v>
       </c>
       <c r="D123" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="E123" s="67" t="s">
-        <v>127</v>
-      </c>
-      <c r="F123" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="G123" s="59" t="s">
-        <v>138</v>
-      </c>
-      <c r="H123" s="67" t="s">
-        <v>108</v>
+        <v>141</v>
+      </c>
+      <c r="E123" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F123" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G123" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="H123" s="59" t="s">
+        <v>102</v>
       </c>
       <c r="I123" s="60" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J123" s="58" t="s">
         <v>41</v>
@@ -6306,15 +6321,15 @@
       <c r="K123" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="L123" s="92"/>
+      <c r="L123" s="81"/>
     </row>
     <row r="124" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A124" s="57">
-        <f t="shared" si="0"/>
+        <f>A123+1</f>
+        <v>11</v>
+      </c>
+      <c r="B124" s="57">
         <v>12</v>
-      </c>
-      <c r="B124" s="57">
-        <v>11</v>
       </c>
       <c r="C124" s="68" t="s">
         <v>174</v>
@@ -6325,10 +6340,10 @@
       <c r="E124" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="F124" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="G124" s="58" t="s">
+      <c r="F124" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G124" s="59" t="s">
         <v>101</v>
       </c>
       <c r="H124" s="59" t="s">
@@ -6338,26 +6353,26 @@
         <v>142</v>
       </c>
       <c r="J124" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="K124" s="58" t="s">
-        <v>140</v>
-      </c>
-      <c r="L124" s="92"/>
+        <v>119</v>
+      </c>
+      <c r="K124" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="L124" s="81"/>
     </row>
     <row r="125" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A125" s="57">
-        <f t="shared" si="0"/>
+        <f>A124+1</f>
+        <v>12</v>
+      </c>
+      <c r="B125" s="57">
         <v>13</v>
-      </c>
-      <c r="B125" s="57">
-        <v>12</v>
       </c>
       <c r="C125" s="68" t="s">
         <v>174</v>
       </c>
       <c r="D125" s="60" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="E125" s="59" t="s">
         <v>111</v>
@@ -6372,29 +6387,29 @@
         <v>102</v>
       </c>
       <c r="I125" s="60" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="J125" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K125" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="L125" s="92"/>
+        <v>41</v>
+      </c>
+      <c r="K125" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="L125" s="81"/>
     </row>
     <row r="126" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A126" s="57">
-        <f t="shared" si="0"/>
+        <f>A125+1</f>
+        <v>13</v>
+      </c>
+      <c r="B126" s="57">
         <v>14</v>
-      </c>
-      <c r="B126" s="57">
-        <v>13</v>
       </c>
       <c r="C126" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="D126" s="60" t="s">
-        <v>122</v>
+      <c r="D126" s="59" t="s">
+        <v>47</v>
       </c>
       <c r="E126" s="59" t="s">
         <v>111</v>
@@ -6408,33 +6423,33 @@
       <c r="H126" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I126" s="60" t="s">
-        <v>123</v>
+      <c r="I126" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="J126" s="58" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="K126" s="58" t="s">
-        <v>144</v>
-      </c>
-      <c r="L126" s="92"/>
+        <v>131</v>
+      </c>
+      <c r="L126" s="81"/>
     </row>
     <row r="127" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A127" s="57">
-        <f t="shared" si="0"/>
+        <f>A126+1</f>
+        <v>14</v>
+      </c>
+      <c r="B127" s="57">
         <v>15</v>
-      </c>
-      <c r="B127" s="57">
-        <v>14</v>
       </c>
       <c r="C127" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="D127" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="E127" s="59" t="s">
-        <v>111</v>
+      <c r="D127" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="E127" s="67" t="s">
+        <v>127</v>
       </c>
       <c r="F127" s="59" t="s">
         <v>107</v>
@@ -6445,33 +6460,33 @@
       <c r="H127" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I127" s="59" t="s">
-        <v>103</v>
+      <c r="I127" s="60" t="s">
+        <v>139</v>
       </c>
       <c r="J127" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K127" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="L127" s="92"/>
-    </row>
-    <row r="128" spans="1:12" s="75" customFormat="1" ht="29.45" customHeight="1">
+        <v>146</v>
+      </c>
+      <c r="L127" s="81"/>
+    </row>
+    <row r="128" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A128" s="57">
-        <f t="shared" si="0"/>
+        <f>A127+1</f>
+        <v>15</v>
+      </c>
+      <c r="B128" s="57">
         <v>16</v>
       </c>
-      <c r="B128" s="57">
-        <v>15</v>
-      </c>
       <c r="C128" s="68" t="s">
-        <v>174</v>
+        <v>63</v>
       </c>
       <c r="D128" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="E128" s="67" t="s">
-        <v>127</v>
+        <v>147</v>
+      </c>
+      <c r="E128" s="60" t="s">
+        <v>148</v>
       </c>
       <c r="F128" s="59" t="s">
         <v>107</v>
@@ -6482,49 +6497,72 @@
       <c r="H128" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I128" s="60" t="s">
-        <v>139</v>
+      <c r="I128" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="J128" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K128" s="58" t="s">
-        <v>146</v>
-      </c>
-      <c r="L128" s="92"/>
+        <v>149</v>
+      </c>
+      <c r="L128" s="81"/>
     </row>
     <row r="129" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A129" s="74">
+      <c r="A129" s="57">
+        <f>A128+1</f>
+        <v>16</v>
+      </c>
+      <c r="B129" s="57">
         <v>17</v>
       </c>
-      <c r="B129" s="74"/>
-      <c r="C129" s="74"/>
-      <c r="D129" s="74"/>
-      <c r="E129" s="74"/>
-      <c r="F129" s="74"/>
-      <c r="G129" s="74"/>
-      <c r="H129" s="74"/>
-      <c r="I129" s="74"/>
-      <c r="J129" s="74"/>
-      <c r="K129" s="74"/>
-      <c r="L129" s="93"/>
+      <c r="C129" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D129" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E129" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="F129" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G129" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H129" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="I129" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="J129" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="K129" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="L129" s="81" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="130" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A130" s="57">
-        <f t="shared" si="0"/>
+        <f>A129+1</f>
+        <v>17</v>
+      </c>
+      <c r="B130" s="57">
         <v>18</v>
-      </c>
-      <c r="B130" s="57">
-        <v>16</v>
       </c>
       <c r="C130" s="68" t="s">
         <v>63</v>
       </c>
       <c r="D130" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="E130" s="60" t="s">
-        <v>148</v>
+        <v>110</v>
+      </c>
+      <c r="E130" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="F130" s="59" t="s">
         <v>107</v>
@@ -6535,72 +6573,51 @@
       <c r="H130" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I130" s="59" t="s">
-        <v>103</v>
+      <c r="I130" s="60" t="s">
+        <v>152</v>
       </c>
       <c r="J130" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K130" s="58" t="s">
-        <v>149</v>
-      </c>
-      <c r="L130" s="92"/>
+        <v>68</v>
+      </c>
+      <c r="L130" s="81" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="131" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A131" s="57">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B131" s="57">
+      <c r="A131" s="72">
         <v>17</v>
       </c>
-      <c r="C131" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="D131" s="60" t="s">
-        <v>105</v>
-      </c>
-      <c r="E131" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="F131" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="G131" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="H131" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="I131" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="J131" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="K131" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="L131" s="92" t="s">
-        <v>151</v>
-      </c>
+      <c r="B131" s="72"/>
+      <c r="C131" s="72"/>
+      <c r="D131" s="72"/>
+      <c r="E131" s="72"/>
+      <c r="F131" s="72"/>
+      <c r="G131" s="72"/>
+      <c r="H131" s="72"/>
+      <c r="I131" s="72"/>
+      <c r="J131" s="72"/>
+      <c r="K131" s="72"/>
+      <c r="L131" s="82"/>
     </row>
     <row r="132" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A132" s="57">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>A131+1</f>
+        <v>18</v>
       </c>
       <c r="B132" s="57">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C132" s="68" t="s">
         <v>63</v>
       </c>
       <c r="D132" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="E132" s="59" t="s">
-        <v>111</v>
+        <v>117</v>
+      </c>
+      <c r="E132" s="67" t="s">
+        <v>127</v>
       </c>
       <c r="F132" s="59" t="s">
         <v>107</v>
@@ -6612,34 +6629,34 @@
         <v>102</v>
       </c>
       <c r="I132" s="60" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J132" s="58" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="K132" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="L132" s="92" t="s">
-        <v>153</v>
+        <v>70</v>
+      </c>
+      <c r="L132" s="81" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="133" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A133" s="57">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f>A132+1</f>
+        <v>19</v>
       </c>
       <c r="B133" s="57">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C133" s="68" t="s">
         <v>63</v>
       </c>
       <c r="D133" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E133" s="67" t="s">
-        <v>127</v>
+        <v>156</v>
+      </c>
+      <c r="E133" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="F133" s="59" t="s">
         <v>107</v>
@@ -6648,34 +6665,32 @@
         <v>101</v>
       </c>
       <c r="H133" s="59" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="I133" s="60" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J133" s="58" t="s">
         <v>41</v>
       </c>
       <c r="K133" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="L133" s="92" t="s">
-        <v>155</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="L133" s="81"/>
     </row>
     <row r="134" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A134" s="57">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f>A133+1</f>
+        <v>20</v>
       </c>
       <c r="B134" s="57">
-        <v>20</v>
-      </c>
-      <c r="C134" s="68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="D134" s="60" t="s">
-        <v>156</v>
+      <c r="D134" s="59" t="s">
+        <v>47</v>
       </c>
       <c r="E134" s="59" t="s">
         <v>111</v>
@@ -6687,32 +6702,32 @@
         <v>101</v>
       </c>
       <c r="H134" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="I134" s="60" t="s">
-        <v>157</v>
+        <v>102</v>
+      </c>
+      <c r="I134" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="J134" s="58" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="K134" s="70" t="s">
-        <v>124</v>
-      </c>
-      <c r="L134" s="92"/>
+        <v>158</v>
+      </c>
+      <c r="L134" s="81"/>
     </row>
     <row r="135" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A135" s="57">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B135" s="90">
+        <f>A134+1</f>
         <v>21</v>
+      </c>
+      <c r="B135" s="79">
+        <v>22</v>
       </c>
       <c r="C135" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D135" s="61" t="s">
-        <v>47</v>
+      <c r="D135" s="62" t="s">
+        <v>126</v>
       </c>
       <c r="E135" s="61" t="s">
         <v>111</v>
@@ -6726,30 +6741,30 @@
       <c r="H135" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I135" s="61" t="s">
-        <v>103</v>
+      <c r="I135" s="62" t="s">
+        <v>159</v>
       </c>
       <c r="J135" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K135" s="70" t="s">
-        <v>158</v>
-      </c>
-      <c r="L135" s="94"/>
+        <v>160</v>
+      </c>
+      <c r="L135" s="83"/>
     </row>
     <row r="136" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A136" s="57">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B136" s="90">
+        <f>A135+1</f>
         <v>22</v>
+      </c>
+      <c r="B136" s="79">
+        <v>23</v>
       </c>
       <c r="C136" s="71" t="s">
         <v>63</v>
       </c>
       <c r="D136" s="60" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="E136" s="61" t="s">
         <v>111</v>
@@ -6764,35 +6779,35 @@
         <v>102</v>
       </c>
       <c r="I136" s="60" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J136" s="58" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="K136" s="70" t="s">
-        <v>160</v>
-      </c>
-      <c r="L136" s="94"/>
-    </row>
-    <row r="137" spans="1:12" s="75" customFormat="1" ht="29.45" customHeight="1">
+        <v>163</v>
+      </c>
+      <c r="L136" s="83"/>
+    </row>
+    <row r="137" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A137" s="57">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B137" s="90">
+        <f>A136+1</f>
         <v>23</v>
       </c>
-      <c r="C137" s="71" t="s">
-        <v>63</v>
+      <c r="B137" s="79">
+        <v>24</v>
+      </c>
+      <c r="C137" s="106" t="s">
+        <v>77</v>
       </c>
       <c r="D137" s="60" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E137" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F137" s="61" t="s">
-        <v>107</v>
+      <c r="F137" s="62" t="s">
+        <v>164</v>
       </c>
       <c r="G137" s="61" t="s">
         <v>101</v>
@@ -6800,159 +6815,157 @@
       <c r="H137" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I137" s="62" t="s">
-        <v>162</v>
+      <c r="I137" s="61" t="s">
+        <v>103</v>
       </c>
       <c r="J137" s="70" t="s">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="K137" s="70" t="s">
-        <v>163</v>
-      </c>
-      <c r="L137" s="94"/>
+        <v>165</v>
+      </c>
+      <c r="L137" s="83"/>
     </row>
     <row r="138" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A138" s="76">
-        <v>26</v>
-      </c>
-      <c r="B138" s="76"/>
-      <c r="C138" s="76"/>
-      <c r="D138" s="76"/>
-      <c r="E138" s="76"/>
-      <c r="F138" s="76"/>
-      <c r="G138" s="76"/>
-      <c r="H138" s="76"/>
-      <c r="I138" s="76"/>
-      <c r="J138" s="76"/>
-      <c r="K138" s="76"/>
-      <c r="L138" s="95"/>
+      <c r="A138" s="79">
+        <f>A137+1</f>
+        <v>24</v>
+      </c>
+      <c r="B138" s="79">
+        <v>25</v>
+      </c>
+      <c r="C138" s="106" t="s">
+        <v>77</v>
+      </c>
+      <c r="D138" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="E138" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F138" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="G138" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H138" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="I138" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="J138" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="K138" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L138" s="83"/>
     </row>
     <row r="139" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A139" s="57">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B139" s="90">
-        <v>24</v>
+        <f>A138+1</f>
+        <v>25</v>
+      </c>
+      <c r="B139" s="79">
+        <v>28</v>
       </c>
       <c r="C139" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D139" s="60" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="E139" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F139" s="62" t="s">
-        <v>164</v>
-      </c>
-      <c r="G139" s="61" t="s">
+      <c r="F139" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G139" s="70" t="s">
         <v>101</v>
       </c>
       <c r="H139" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I139" s="61" t="s">
-        <v>103</v>
-      </c>
-      <c r="J139" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="K139" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="L139" s="94"/>
+      <c r="I139" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="J139" s="107" t="s">
+        <v>41</v>
+      </c>
+      <c r="K139" s="107" t="s">
+        <v>173</v>
+      </c>
+      <c r="L139" s="83"/>
     </row>
     <row r="140" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A140" s="57">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B140" s="90">
-        <v>25</v>
+        <f>A139+1</f>
+        <v>26</v>
+      </c>
+      <c r="B140" s="79">
+        <v>29</v>
       </c>
       <c r="C140" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="D140" s="60" t="s">
-        <v>105</v>
+      <c r="D140" s="59" t="s">
+        <v>47</v>
       </c>
       <c r="E140" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F140" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="G140" s="61" t="s">
+      <c r="F140" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="G140" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="H140" s="60" t="s">
-        <v>108</v>
+      <c r="H140" s="59" t="s">
+        <v>102</v>
       </c>
       <c r="I140" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="J140" s="70" t="s">
+      <c r="J140" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="K140" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="L140" s="94"/>
+      <c r="K140" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="L140" s="83"/>
     </row>
     <row r="141" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A141" s="57">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B141" s="90">
+      <c r="A141" s="72">
         <v>26</v>
       </c>
-      <c r="C141" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="D141" s="60" t="s">
-        <v>166</v>
-      </c>
-      <c r="E141" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="F141" s="61" t="s">
-        <v>107</v>
-      </c>
-      <c r="G141" s="66" t="s">
-        <v>167</v>
-      </c>
-      <c r="H141" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="I141" s="60" t="s">
-        <v>168</v>
-      </c>
-      <c r="J141" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K141" s="61" t="s">
-        <v>169</v>
-      </c>
-      <c r="L141" s="94" t="s">
-        <v>170</v>
-      </c>
+      <c r="B141" s="74"/>
+      <c r="C141" s="72"/>
+      <c r="D141" s="72"/>
+      <c r="E141" s="74"/>
+      <c r="F141" s="74"/>
+      <c r="G141" s="74"/>
+      <c r="H141" s="74"/>
+      <c r="I141" s="72"/>
+      <c r="J141" s="72"/>
+      <c r="K141" s="74"/>
+      <c r="L141" s="84"/>
     </row>
     <row r="142" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A142" s="57">
-        <f t="shared" si="0"/>
+        <f>A141+1</f>
+        <v>27</v>
+      </c>
+      <c r="B142" s="79">
         <v>30</v>
-      </c>
-      <c r="B142" s="90">
-        <v>27</v>
       </c>
       <c r="C142" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D142" s="60" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E142" s="61" t="s">
         <v>111</v>
@@ -6960,36 +6973,36 @@
       <c r="F142" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="G142" s="66" t="s">
-        <v>167</v>
+      <c r="G142" s="70" t="s">
+        <v>101</v>
       </c>
       <c r="H142" s="61" t="s">
         <v>102</v>
       </c>
       <c r="I142" s="60" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="J142" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="K142" s="72" t="s">
-        <v>171</v>
-      </c>
-      <c r="L142" s="94"/>
+      <c r="K142" s="108" t="s">
+        <v>89</v>
+      </c>
+      <c r="L142" s="83"/>
     </row>
     <row r="143" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A143" s="57">
-        <f t="shared" si="0"/>
+        <f>A142+1</f>
+        <v>28</v>
+      </c>
+      <c r="B143" s="79">
         <v>31</v>
-      </c>
-      <c r="B143" s="90">
-        <v>28</v>
       </c>
       <c r="C143" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D143" s="60" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="E143" s="61" t="s">
         <v>111</v>
@@ -7004,29 +7017,29 @@
         <v>102</v>
       </c>
       <c r="I143" s="60" t="s">
-        <v>172</v>
-      </c>
-      <c r="J143" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="K143" s="72" t="s">
-        <v>173</v>
-      </c>
-      <c r="L143" s="94"/>
+        <v>162</v>
+      </c>
+      <c r="J143" s="108" t="s">
+        <v>15</v>
+      </c>
+      <c r="K143" s="108" t="s">
+        <v>90</v>
+      </c>
+      <c r="L143" s="83"/>
     </row>
     <row r="144" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A144" s="57">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B144" s="90">
+        <f>A143+1</f>
         <v>29</v>
+      </c>
+      <c r="B144" s="79">
+        <v>26</v>
       </c>
       <c r="C144" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="D144" s="59" t="s">
-        <v>47</v>
+      <c r="D144" s="60" t="s">
+        <v>166</v>
       </c>
       <c r="E144" s="61" t="s">
         <v>111</v>
@@ -7034,36 +7047,38 @@
       <c r="F144" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="G144" s="58" t="s">
-        <v>101</v>
+      <c r="G144" s="67" t="s">
+        <v>167</v>
       </c>
       <c r="H144" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I144" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="J144" s="73" t="s">
-        <v>15</v>
-      </c>
-      <c r="K144" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="L144" s="94"/>
+      <c r="I144" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="J144" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="K144" s="108" t="s">
+        <v>169</v>
+      </c>
+      <c r="L144" s="83" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="145" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A145" s="57">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B145" s="90">
+        <f>A144+1</f>
         <v>30</v>
+      </c>
+      <c r="B145" s="79">
+        <v>27</v>
       </c>
       <c r="C145" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D145" s="60" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E145" s="61" t="s">
         <v>111</v>
@@ -7071,59 +7086,59 @@
       <c r="F145" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="G145" s="58" t="s">
-        <v>101</v>
+      <c r="G145" s="67" t="s">
+        <v>167</v>
       </c>
       <c r="H145" s="61" t="s">
         <v>102</v>
       </c>
       <c r="I145" s="60" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="J145" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="K145" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="L145" s="94"/>
-    </row>
-    <row r="146" spans="1:12" ht="30">
+      <c r="K145" s="107" t="s">
+        <v>171</v>
+      </c>
+      <c r="L145" s="83"/>
+    </row>
+    <row r="146" spans="1:12" ht="15">
       <c r="A146" s="57">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B146" s="97">
+        <f>A145+1</f>
         <v>31</v>
       </c>
-      <c r="C146" s="98" t="s">
-        <v>77</v>
-      </c>
-      <c r="D146" s="99" t="s">
-        <v>161</v>
-      </c>
-      <c r="E146" s="100" t="s">
-        <v>111</v>
-      </c>
-      <c r="F146" s="100" t="s">
+      <c r="B146" s="86">
+        <v>10</v>
+      </c>
+      <c r="C146" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="D146" s="88" t="s">
+        <v>137</v>
+      </c>
+      <c r="E146" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F146" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="G146" s="101" t="s">
-        <v>101</v>
-      </c>
-      <c r="H146" s="100" t="s">
-        <v>102</v>
-      </c>
-      <c r="I146" s="102" t="s">
-        <v>162</v>
-      </c>
-      <c r="J146" s="103" t="s">
-        <v>15</v>
-      </c>
-      <c r="K146" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="L146" s="104"/>
+      <c r="G146" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="H146" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="I146" s="91" t="s">
+        <v>139</v>
+      </c>
+      <c r="J146" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="K146" s="110" t="s">
+        <v>140</v>
+      </c>
+      <c r="L146" s="93"/>
     </row>
     <row r="147" spans="1:12" ht="15">
       <c r="A147" s="54"/>
@@ -7177,6 +7192,8 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C111:J111"/>
+    <mergeCell ref="C108:F108"/>
     <mergeCell ref="C109:F109"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
@@ -7185,11 +7202,9 @@
     <mergeCell ref="A108:A109"/>
     <mergeCell ref="G108:G109"/>
     <mergeCell ref="H108:H109"/>
-    <mergeCell ref="C111:J111"/>
-    <mergeCell ref="C108:F108"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:I104 C130:C146">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Codage Scenarios Excel to CCSL (1/4)
En espérant qu'ils soient bon pour notre encadrant!
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1555C257-378B-4832-819D-493D4AD5BD06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284F46A3-2623-4F1C-8506-722C883B7F60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="21495" yWindow="10215" windowWidth="7650" windowHeight="4650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,25 +573,30 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -818,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1067,11 +1072,20 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1092,28 +1106,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1777,8 +1779,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K119" sqref="K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1793,31 +1795,32 @@
     <col min="9" max="9" width="29" customWidth="1"/>
     <col min="10" max="10" width="37.85546875" customWidth="1"/>
     <col min="11" max="11" width="94" customWidth="1"/>
+    <col min="12" max="12" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="95" t="s">
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="98" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="103" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A2" s="96"/>
+      <c r="A2" s="99"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1833,11 +1836,11 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="96"/>
+      <c r="G2" s="99"/>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="96"/>
+      <c r="I2" s="99"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" hidden="1" customHeight="1">
       <c r="A3" s="3"/>
@@ -5851,26 +5854,26 @@
       <c r="AB107" s="53"/>
     </row>
     <row r="108" spans="1:28" ht="15">
-      <c r="A108" s="94"/>
-      <c r="C108" s="94" t="s">
+      <c r="A108" s="97"/>
+      <c r="C108" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="D108" s="94"/>
-      <c r="E108" s="94"/>
-      <c r="F108" s="94"/>
-      <c r="G108" s="94"/>
-      <c r="H108" s="102"/>
+      <c r="D108" s="97"/>
+      <c r="E108" s="97"/>
+      <c r="F108" s="97"/>
+      <c r="G108" s="97"/>
+      <c r="H108" s="105"/>
     </row>
     <row r="109" spans="1:28" ht="15">
-      <c r="A109" s="101"/>
-      <c r="C109" s="94" t="s">
+      <c r="A109" s="104"/>
+      <c r="C109" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="D109" s="94"/>
-      <c r="E109" s="94"/>
-      <c r="F109" s="94"/>
-      <c r="G109" s="101"/>
-      <c r="H109" s="101"/>
+      <c r="D109" s="97"/>
+      <c r="E109" s="97"/>
+      <c r="F109" s="97"/>
+      <c r="G109" s="104"/>
+      <c r="H109" s="104"/>
     </row>
     <row r="110" spans="1:28" s="76" customFormat="1" ht="15">
       <c r="B110" s="75"/>
@@ -5879,16 +5882,16 @@
     </row>
     <row r="111" spans="1:28" ht="15">
       <c r="A111" s="54"/>
-      <c r="C111" s="103" t="s">
+      <c r="C111" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D111" s="104"/>
-      <c r="E111" s="104"/>
-      <c r="F111" s="104"/>
-      <c r="G111" s="104"/>
-      <c r="H111" s="104"/>
-      <c r="I111" s="104"/>
-      <c r="J111" s="104"/>
+      <c r="D111" s="96"/>
+      <c r="E111" s="96"/>
+      <c r="F111" s="96"/>
+      <c r="G111" s="96"/>
+      <c r="H111" s="96"/>
+      <c r="I111" s="96"/>
+      <c r="J111" s="96"/>
     </row>
     <row r="112" spans="1:28" ht="15">
       <c r="A112" s="78" t="s">
@@ -6196,61 +6199,59 @@
     </row>
     <row r="120" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A120" s="57">
-        <f>A119+1</f>
         <v>8</v>
       </c>
-      <c r="B120" s="57">
+      <c r="B120" s="72"/>
+      <c r="C120" s="72"/>
+      <c r="D120" s="72"/>
+      <c r="E120" s="72"/>
+      <c r="F120" s="72"/>
+      <c r="G120" s="72"/>
+      <c r="H120" s="72"/>
+      <c r="I120" s="72"/>
+      <c r="J120" s="72"/>
+      <c r="K120" s="72"/>
+      <c r="L120" s="82"/>
+    </row>
+    <row r="121" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A121" s="57">
+        <v>9</v>
+      </c>
+      <c r="B121" s="57">
         <v>8</v>
       </c>
-      <c r="C120" s="68" t="s">
+      <c r="C121" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="D120" s="60" t="s">
+      <c r="D121" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="E120" s="60" t="s">
+      <c r="E121" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="F120" s="59" t="s">
+      <c r="F121" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="G120" s="59" t="s">
+      <c r="G121" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="H120" s="59" t="s">
+      <c r="H121" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I120" s="59" t="s">
+      <c r="I121" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="J120" s="58" t="s">
+      <c r="J121" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="K120" s="58" t="s">
+      <c r="K121" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="L120" s="81"/>
-    </row>
-    <row r="121" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A121" s="72">
-        <v>8</v>
-      </c>
-      <c r="B121" s="72"/>
-      <c r="C121" s="72"/>
-      <c r="D121" s="72"/>
-      <c r="E121" s="72"/>
-      <c r="F121" s="72"/>
-      <c r="G121" s="72"/>
-      <c r="H121" s="72"/>
-      <c r="I121" s="72"/>
-      <c r="J121" s="72"/>
-      <c r="K121" s="72"/>
-      <c r="L121" s="82"/>
+      <c r="L121" s="81"/>
     </row>
     <row r="122" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A122" s="57">
-        <f>A121+1</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B122" s="57">
         <v>9</v>
@@ -6288,32 +6289,31 @@
     </row>
     <row r="123" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A123" s="57">
-        <f>A122+1</f>
+        <v>11</v>
+      </c>
+      <c r="B123" s="57">
         <v>10</v>
-      </c>
-      <c r="B123" s="57">
-        <v>11</v>
       </c>
       <c r="C123" s="68" t="s">
         <v>174</v>
       </c>
       <c r="D123" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="E123" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="F123" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="G123" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="H123" s="59" t="s">
-        <v>102</v>
+        <v>137</v>
+      </c>
+      <c r="E123" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="F123" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G123" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="H123" s="67" t="s">
+        <v>108</v>
       </c>
       <c r="I123" s="60" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J123" s="58" t="s">
         <v>41</v>
@@ -6325,11 +6325,10 @@
     </row>
     <row r="124" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A124" s="57">
-        <f>A123+1</f>
+        <v>12</v>
+      </c>
+      <c r="B124" s="57">
         <v>11</v>
-      </c>
-      <c r="B124" s="57">
-        <v>12</v>
       </c>
       <c r="C124" s="68" t="s">
         <v>174</v>
@@ -6340,10 +6339,10 @@
       <c r="E124" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="F124" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="G124" s="59" t="s">
+      <c r="F124" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G124" s="58" t="s">
         <v>101</v>
       </c>
       <c r="H124" s="59" t="s">
@@ -6353,26 +6352,26 @@
         <v>142</v>
       </c>
       <c r="J124" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K124" s="59" t="s">
-        <v>143</v>
+        <v>41</v>
+      </c>
+      <c r="K124" s="58" t="s">
+        <v>140</v>
       </c>
       <c r="L124" s="81"/>
     </row>
     <row r="125" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A125" s="57">
         <f>A124+1</f>
+        <v>13</v>
+      </c>
+      <c r="B125" s="57">
         <v>12</v>
-      </c>
-      <c r="B125" s="57">
-        <v>13</v>
       </c>
       <c r="C125" s="68" t="s">
         <v>174</v>
       </c>
       <c r="D125" s="60" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="E125" s="59" t="s">
         <v>111</v>
@@ -6387,29 +6386,29 @@
         <v>102</v>
       </c>
       <c r="I125" s="60" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="J125" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="K125" s="58" t="s">
-        <v>144</v>
+        <v>119</v>
+      </c>
+      <c r="K125" s="59" t="s">
+        <v>143</v>
       </c>
       <c r="L125" s="81"/>
     </row>
     <row r="126" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A126" s="57">
         <f>A125+1</f>
+        <v>14</v>
+      </c>
+      <c r="B126" s="57">
         <v>13</v>
-      </c>
-      <c r="B126" s="57">
-        <v>14</v>
       </c>
       <c r="C126" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="D126" s="59" t="s">
-        <v>47</v>
+      <c r="D126" s="60" t="s">
+        <v>122</v>
       </c>
       <c r="E126" s="59" t="s">
         <v>111</v>
@@ -6423,33 +6422,33 @@
       <c r="H126" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I126" s="59" t="s">
-        <v>103</v>
+      <c r="I126" s="60" t="s">
+        <v>123</v>
       </c>
       <c r="J126" s="58" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="K126" s="58" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="L126" s="81"/>
     </row>
     <row r="127" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A127" s="57">
         <f>A126+1</f>
+        <v>15</v>
+      </c>
+      <c r="B127" s="57">
         <v>14</v>
-      </c>
-      <c r="B127" s="57">
-        <v>15</v>
       </c>
       <c r="C127" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="D127" s="60" t="s">
-        <v>145</v>
-      </c>
-      <c r="E127" s="67" t="s">
-        <v>127</v>
+      <c r="D127" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E127" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="F127" s="59" t="s">
         <v>107</v>
@@ -6460,33 +6459,33 @@
       <c r="H127" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I127" s="60" t="s">
-        <v>139</v>
+      <c r="I127" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="J127" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K127" s="58" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="L127" s="81"/>
     </row>
     <row r="128" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A128" s="57">
         <f>A127+1</f>
+        <v>16</v>
+      </c>
+      <c r="B128" s="57">
         <v>15</v>
       </c>
-      <c r="B128" s="57">
-        <v>16</v>
-      </c>
       <c r="C128" s="68" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="D128" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="E128" s="60" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="E128" s="67" t="s">
+        <v>127</v>
       </c>
       <c r="F128" s="59" t="s">
         <v>107</v>
@@ -6497,72 +6496,49 @@
       <c r="H128" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I128" s="59" t="s">
-        <v>103</v>
+      <c r="I128" s="60" t="s">
+        <v>139</v>
       </c>
       <c r="J128" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K128" s="58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L128" s="81"/>
     </row>
     <row r="129" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A129" s="57">
-        <f>A128+1</f>
-        <v>16</v>
-      </c>
-      <c r="B129" s="57">
         <v>17</v>
       </c>
-      <c r="C129" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="D129" s="60" t="s">
-        <v>105</v>
-      </c>
-      <c r="E129" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="F129" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="G129" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="H129" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="I129" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="J129" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="K129" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="L129" s="81" t="s">
-        <v>151</v>
-      </c>
+      <c r="B129" s="72"/>
+      <c r="C129" s="72"/>
+      <c r="D129" s="72"/>
+      <c r="E129" s="72"/>
+      <c r="F129" s="72"/>
+      <c r="G129" s="72"/>
+      <c r="H129" s="72"/>
+      <c r="I129" s="72"/>
+      <c r="J129" s="72"/>
+      <c r="K129" s="72"/>
+      <c r="L129" s="82"/>
     </row>
     <row r="130" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A130" s="57">
         <f>A129+1</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B130" s="57">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C130" s="68" t="s">
         <v>63</v>
       </c>
       <c r="D130" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="E130" s="59" t="s">
-        <v>111</v>
+        <v>147</v>
+      </c>
+      <c r="E130" s="60" t="s">
+        <v>148</v>
       </c>
       <c r="F130" s="59" t="s">
         <v>107</v>
@@ -6573,51 +6549,72 @@
       <c r="H130" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I130" s="60" t="s">
-        <v>152</v>
+      <c r="I130" s="59" t="s">
+        <v>103</v>
       </c>
       <c r="J130" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K130" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="L130" s="81" t="s">
-        <v>153</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="L130" s="81"/>
     </row>
     <row r="131" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A131" s="72">
+      <c r="A131" s="57">
+        <f>A130+1</f>
+        <v>19</v>
+      </c>
+      <c r="B131" s="57">
         <v>17</v>
       </c>
-      <c r="B131" s="72"/>
-      <c r="C131" s="72"/>
-      <c r="D131" s="72"/>
-      <c r="E131" s="72"/>
-      <c r="F131" s="72"/>
-      <c r="G131" s="72"/>
-      <c r="H131" s="72"/>
-      <c r="I131" s="72"/>
-      <c r="J131" s="72"/>
-      <c r="K131" s="72"/>
-      <c r="L131" s="82"/>
+      <c r="C131" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D131" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E131" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="F131" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="G131" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="H131" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="I131" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="J131" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="K131" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="L131" s="81" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="132" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A132" s="57">
         <f>A131+1</f>
+        <v>20</v>
+      </c>
+      <c r="B132" s="57">
         <v>18</v>
-      </c>
-      <c r="B132" s="57">
-        <v>19</v>
       </c>
       <c r="C132" s="68" t="s">
         <v>63</v>
       </c>
       <c r="D132" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E132" s="67" t="s">
-        <v>127</v>
+        <v>105</v>
+      </c>
+      <c r="E132" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="F132" s="59" t="s">
         <v>107</v>
@@ -6625,29 +6622,29 @@
       <c r="G132" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="H132" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="I132" s="60" t="s">
-        <v>154</v>
+      <c r="H132" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="I132" s="67" t="s">
+        <v>150</v>
       </c>
       <c r="J132" s="58" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="K132" s="58" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="L132" s="81" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="133" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A133" s="57">
         <f>A132+1</f>
+        <v>21</v>
+      </c>
+      <c r="B133" s="57">
         <v>19</v>
-      </c>
-      <c r="B133" s="57">
-        <v>20</v>
       </c>
       <c r="C133" s="68" t="s">
         <v>63</v>
@@ -6681,16 +6678,16 @@
     <row r="134" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A134" s="57">
         <f>A133+1</f>
+        <v>22</v>
+      </c>
+      <c r="B134" s="57">
         <v>20</v>
       </c>
-      <c r="B134" s="57">
-        <v>21</v>
-      </c>
-      <c r="C134" s="105" t="s">
+      <c r="C134" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D134" s="59" t="s">
-        <v>47</v>
+      <c r="D134" s="60" t="s">
+        <v>110</v>
       </c>
       <c r="E134" s="59" t="s">
         <v>111</v>
@@ -6704,30 +6701,32 @@
       <c r="H134" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I134" s="59" t="s">
-        <v>103</v>
+      <c r="I134" s="60" t="s">
+        <v>152</v>
       </c>
       <c r="J134" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K134" s="70" t="s">
-        <v>158</v>
-      </c>
-      <c r="L134" s="81"/>
+        <v>68</v>
+      </c>
+      <c r="L134" s="81" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="135" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A135" s="57">
         <f>A134+1</f>
+        <v>23</v>
+      </c>
+      <c r="B135" s="79">
         <v>21</v>
-      </c>
-      <c r="B135" s="79">
-        <v>22</v>
       </c>
       <c r="C135" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="D135" s="62" t="s">
-        <v>126</v>
+      <c r="D135" s="61" t="s">
+        <v>47</v>
       </c>
       <c r="E135" s="61" t="s">
         <v>111</v>
@@ -6741,30 +6740,30 @@
       <c r="H135" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I135" s="62" t="s">
-        <v>159</v>
+      <c r="I135" s="61" t="s">
+        <v>103</v>
       </c>
       <c r="J135" s="58" t="s">
         <v>119</v>
       </c>
       <c r="K135" s="70" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="L135" s="83"/>
     </row>
     <row r="136" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A136" s="57">
         <f>A135+1</f>
+        <v>24</v>
+      </c>
+      <c r="B136" s="79">
         <v>22</v>
-      </c>
-      <c r="B136" s="79">
-        <v>23</v>
       </c>
       <c r="C136" s="71" t="s">
         <v>63</v>
       </c>
       <c r="D136" s="60" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="E136" s="61" t="s">
         <v>111</v>
@@ -6779,35 +6778,35 @@
         <v>102</v>
       </c>
       <c r="I136" s="60" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J136" s="58" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="K136" s="70" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L136" s="83"/>
     </row>
     <row r="137" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A137" s="57">
         <f>A136+1</f>
+        <v>25</v>
+      </c>
+      <c r="B137" s="79">
         <v>23</v>
       </c>
-      <c r="B137" s="79">
-        <v>24</v>
-      </c>
-      <c r="C137" s="106" t="s">
-        <v>77</v>
+      <c r="C137" s="71" t="s">
+        <v>63</v>
       </c>
       <c r="D137" s="60" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E137" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F137" s="62" t="s">
-        <v>164</v>
+      <c r="F137" s="61" t="s">
+        <v>107</v>
       </c>
       <c r="G137" s="61" t="s">
         <v>101</v>
@@ -6815,104 +6814,83 @@
       <c r="H137" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I137" s="61" t="s">
-        <v>103</v>
+      <c r="I137" s="62" t="s">
+        <v>162</v>
       </c>
       <c r="J137" s="70" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="K137" s="70" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L137" s="83"/>
     </row>
     <row r="138" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A138" s="79">
-        <f>A137+1</f>
-        <v>24</v>
-      </c>
-      <c r="B138" s="79">
-        <v>25</v>
-      </c>
-      <c r="C138" s="106" t="s">
-        <v>77</v>
-      </c>
-      <c r="D138" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="E138" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="F138" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="G138" s="61" t="s">
-        <v>101</v>
-      </c>
-      <c r="H138" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="I138" s="61" t="s">
-        <v>103</v>
-      </c>
-      <c r="J138" s="70" t="s">
-        <v>15</v>
-      </c>
-      <c r="K138" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="L138" s="83"/>
+        <v>26</v>
+      </c>
+      <c r="B138" s="74"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="74"/>
+      <c r="E138" s="74"/>
+      <c r="F138" s="74"/>
+      <c r="G138" s="74"/>
+      <c r="H138" s="74"/>
+      <c r="I138" s="74"/>
+      <c r="J138" s="74"/>
+      <c r="K138" s="74"/>
+      <c r="L138" s="84"/>
     </row>
     <row r="139" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A139" s="57">
         <f>A138+1</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B139" s="79">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C139" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D139" s="60" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="E139" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="F139" s="61" t="s">
-        <v>107</v>
-      </c>
-      <c r="G139" s="70" t="s">
+      <c r="F139" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="G139" s="61" t="s">
         <v>101</v>
       </c>
       <c r="H139" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I139" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="J139" s="107" t="s">
-        <v>41</v>
-      </c>
-      <c r="K139" s="107" t="s">
-        <v>173</v>
+      <c r="I139" s="61" t="s">
+        <v>103</v>
+      </c>
+      <c r="J139" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="K139" s="70" t="s">
+        <v>165</v>
       </c>
       <c r="L139" s="83"/>
     </row>
     <row r="140" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A140" s="57">
         <f>A139+1</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B140" s="79">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C140" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="D140" s="59" t="s">
-        <v>47</v>
+      <c r="D140" s="60" t="s">
+        <v>126</v>
       </c>
       <c r="E140" s="61" t="s">
         <v>111</v>
@@ -6926,46 +6904,67 @@
       <c r="H140" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="I140" s="61" t="s">
+      <c r="I140" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="J140" s="70" t="s">
+        <v>119</v>
+      </c>
+      <c r="K140" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="L140" s="83"/>
+    </row>
+    <row r="141" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
+      <c r="A141" s="57">
+        <f>A140+1</f>
+        <v>29</v>
+      </c>
+      <c r="B141" s="79">
+        <v>26</v>
+      </c>
+      <c r="C141" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D141" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E141" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="F141" s="66" t="s">
+        <v>164</v>
+      </c>
+      <c r="G141" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H141" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="I141" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="J140" s="107" t="s">
+      <c r="J141" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="K140" s="107" t="s">
-        <v>48</v>
-      </c>
-      <c r="L140" s="83"/>
-    </row>
-    <row r="141" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
-      <c r="A141" s="72">
-        <v>26</v>
-      </c>
-      <c r="B141" s="74"/>
-      <c r="C141" s="72"/>
-      <c r="D141" s="72"/>
-      <c r="E141" s="74"/>
-      <c r="F141" s="74"/>
-      <c r="G141" s="74"/>
-      <c r="H141" s="74"/>
-      <c r="I141" s="72"/>
-      <c r="J141" s="72"/>
-      <c r="K141" s="74"/>
-      <c r="L141" s="84"/>
+      <c r="K141" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="L141" s="83"/>
     </row>
     <row r="142" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A142" s="57">
         <f>A141+1</f>
+        <v>30</v>
+      </c>
+      <c r="B142" s="79">
         <v>27</v>
-      </c>
-      <c r="B142" s="79">
-        <v>30</v>
       </c>
       <c r="C142" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D142" s="60" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="E142" s="61" t="s">
         <v>111</v>
@@ -6980,29 +6979,29 @@
         <v>102</v>
       </c>
       <c r="I142" s="60" t="s">
-        <v>159</v>
-      </c>
-      <c r="J142" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K142" s="108" t="s">
-        <v>89</v>
+        <v>162</v>
+      </c>
+      <c r="J142" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K142" s="94" t="s">
+        <v>90</v>
       </c>
       <c r="L142" s="83"/>
     </row>
     <row r="143" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A143" s="57">
         <f>A142+1</f>
+        <v>31</v>
+      </c>
+      <c r="B143" s="79">
         <v>28</v>
-      </c>
-      <c r="B143" s="79">
-        <v>31</v>
       </c>
       <c r="C143" s="68" t="s">
         <v>77</v>
       </c>
       <c r="D143" s="60" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="E143" s="61" t="s">
         <v>111</v>
@@ -7017,23 +7016,23 @@
         <v>102</v>
       </c>
       <c r="I143" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="J143" s="108" t="s">
-        <v>15</v>
-      </c>
-      <c r="K143" s="108" t="s">
-        <v>90</v>
+        <v>172</v>
+      </c>
+      <c r="J143" s="109" t="s">
+        <v>41</v>
+      </c>
+      <c r="K143" s="109" t="s">
+        <v>173</v>
       </c>
       <c r="L143" s="83"/>
     </row>
     <row r="144" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A144" s="57">
         <f>A143+1</f>
+        <v>32</v>
+      </c>
+      <c r="B144" s="79">
         <v>29</v>
-      </c>
-      <c r="B144" s="79">
-        <v>26</v>
       </c>
       <c r="C144" s="68" t="s">
         <v>77</v>
@@ -7059,7 +7058,7 @@
       <c r="J144" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="K144" s="108" t="s">
+      <c r="K144" s="94" t="s">
         <v>169</v>
       </c>
       <c r="L144" s="83" t="s">
@@ -7069,16 +7068,16 @@
     <row r="145" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A145" s="57">
         <f>A144+1</f>
+        <v>33</v>
+      </c>
+      <c r="B145" s="79">
         <v>30</v>
-      </c>
-      <c r="B145" s="79">
-        <v>27</v>
       </c>
       <c r="C145" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="D145" s="60" t="s">
-        <v>141</v>
+      <c r="D145" s="59" t="s">
+        <v>47</v>
       </c>
       <c r="E145" s="61" t="s">
         <v>111</v>
@@ -7086,59 +7085,59 @@
       <c r="F145" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="G145" s="67" t="s">
-        <v>167</v>
+      <c r="G145" s="58" t="s">
+        <v>101</v>
       </c>
       <c r="H145" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="I145" s="60" t="s">
-        <v>142</v>
-      </c>
-      <c r="J145" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="K145" s="107" t="s">
-        <v>171</v>
+      <c r="I145" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="J145" s="107" t="s">
+        <v>15</v>
+      </c>
+      <c r="K145" s="93" t="s">
+        <v>48</v>
       </c>
       <c r="L145" s="83"/>
     </row>
-    <row r="146" spans="1:12" ht="15">
+    <row r="146" spans="1:12" ht="30">
       <c r="A146" s="57">
         <f>A145+1</f>
+        <v>34</v>
+      </c>
+      <c r="B146" s="86">
         <v>31</v>
       </c>
-      <c r="B146" s="86">
-        <v>10</v>
-      </c>
       <c r="C146" s="87" t="s">
-        <v>174</v>
+        <v>77</v>
       </c>
       <c r="D146" s="88" t="s">
-        <v>137</v>
-      </c>
-      <c r="E146" s="109" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="E146" s="89" t="s">
+        <v>111</v>
       </c>
       <c r="F146" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="G146" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="H146" s="109" t="s">
-        <v>108</v>
+      <c r="G146" s="106" t="s">
+        <v>167</v>
+      </c>
+      <c r="H146" s="89" t="s">
+        <v>102</v>
       </c>
       <c r="I146" s="91" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J146" s="90" t="s">
-        <v>41</v>
-      </c>
-      <c r="K146" s="110" t="s">
-        <v>140</v>
-      </c>
-      <c r="L146" s="93"/>
+        <v>119</v>
+      </c>
+      <c r="K146" s="108" t="s">
+        <v>171</v>
+      </c>
+      <c r="L146" s="92"/>
     </row>
     <row r="147" spans="1:12" ht="15">
       <c r="A147" s="54"/>

</xml_diff>

<commit_message>
Changement ID, Refactor et Redeplacement
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284F46A3-2623-4F1C-8506-722C883B7F60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6637D499-D487-4DE6-9E68-132D195B97FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="21495" yWindow="10215" windowWidth="7650" windowHeight="4650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="210">
   <si>
     <t>ID</t>
   </si>
@@ -557,6 +557,99 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
   </si>
 </sst>
 </file>
@@ -1081,6 +1174,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1105,18 +1210,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1779,8 +1872,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K119" sqref="K119"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1799,28 +1892,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="98" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="102" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="107" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="15.75" hidden="1" customHeight="1">
-      <c r="A2" s="99"/>
+      <c r="A2" s="103"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1836,11 +1929,11 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="99"/>
+      <c r="G2" s="103"/>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="99"/>
+      <c r="I2" s="103"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" hidden="1" customHeight="1">
       <c r="A3" s="3"/>
@@ -5854,26 +5947,26 @@
       <c r="AB107" s="53"/>
     </row>
     <row r="108" spans="1:28" ht="15">
-      <c r="A108" s="97"/>
-      <c r="C108" s="97" t="s">
+      <c r="A108" s="101"/>
+      <c r="C108" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="D108" s="97"/>
-      <c r="E108" s="97"/>
-      <c r="F108" s="97"/>
-      <c r="G108" s="97"/>
-      <c r="H108" s="105"/>
+      <c r="D108" s="101"/>
+      <c r="E108" s="101"/>
+      <c r="F108" s="101"/>
+      <c r="G108" s="101"/>
+      <c r="H108" s="109"/>
     </row>
     <row r="109" spans="1:28" ht="15">
-      <c r="A109" s="104"/>
-      <c r="C109" s="97" t="s">
+      <c r="A109" s="108"/>
+      <c r="C109" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="D109" s="97"/>
-      <c r="E109" s="97"/>
-      <c r="F109" s="97"/>
-      <c r="G109" s="104"/>
-      <c r="H109" s="104"/>
+      <c r="D109" s="101"/>
+      <c r="E109" s="101"/>
+      <c r="F109" s="101"/>
+      <c r="G109" s="108"/>
+      <c r="H109" s="108"/>
     </row>
     <row r="110" spans="1:28" s="76" customFormat="1" ht="15">
       <c r="B110" s="75"/>
@@ -5882,16 +5975,16 @@
     </row>
     <row r="111" spans="1:28" ht="15">
       <c r="A111" s="54"/>
-      <c r="C111" s="95" t="s">
+      <c r="C111" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="D111" s="96"/>
-      <c r="E111" s="96"/>
-      <c r="F111" s="96"/>
-      <c r="G111" s="96"/>
-      <c r="H111" s="96"/>
-      <c r="I111" s="96"/>
-      <c r="J111" s="96"/>
+      <c r="D111" s="100"/>
+      <c r="E111" s="100"/>
+      <c r="F111" s="100"/>
+      <c r="G111" s="100"/>
+      <c r="H111" s="100"/>
+      <c r="I111" s="100"/>
+      <c r="J111" s="100"/>
     </row>
     <row r="112" spans="1:28" ht="15">
       <c r="A112" s="78" t="s">
@@ -5935,8 +6028,8 @@
       <c r="A113" s="57">
         <v>1</v>
       </c>
-      <c r="B113" s="57">
-        <v>1</v>
+      <c r="B113" s="57" t="s">
+        <v>179</v>
       </c>
       <c r="C113" s="68" t="s">
         <v>11</v>
@@ -5969,11 +6062,11 @@
     </row>
     <row r="114" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A114" s="57">
-        <f>A113+1</f>
+        <f t="shared" ref="A114:A119" si="0">A113+1</f>
         <v>2</v>
       </c>
-      <c r="B114" s="57">
-        <v>2</v>
+      <c r="B114" s="57" t="s">
+        <v>180</v>
       </c>
       <c r="C114" s="68" t="s">
         <v>11</v>
@@ -6006,11 +6099,11 @@
     </row>
     <row r="115" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A115" s="57">
-        <f>A114+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B115" s="57">
-        <v>3</v>
+      <c r="B115" s="57" t="s">
+        <v>181</v>
       </c>
       <c r="C115" s="68" t="s">
         <v>11</v>
@@ -6045,11 +6138,11 @@
     </row>
     <row r="116" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A116" s="57">
-        <f>A115+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B116" s="57">
-        <v>4</v>
+      <c r="B116" s="57" t="s">
+        <v>182</v>
       </c>
       <c r="C116" s="68" t="s">
         <v>11</v>
@@ -6084,11 +6177,11 @@
     </row>
     <row r="117" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A117" s="57">
-        <f>A116+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B117" s="57">
-        <v>5</v>
+      <c r="B117" s="57" t="s">
+        <v>183</v>
       </c>
       <c r="C117" s="68" t="s">
         <v>11</v>
@@ -6123,11 +6216,11 @@
     </row>
     <row r="118" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A118" s="57">
-        <f>A117+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B118" s="59">
-        <v>6</v>
+      <c r="B118" s="59" t="s">
+        <v>184</v>
       </c>
       <c r="C118" s="68" t="s">
         <v>11</v>
@@ -6162,11 +6255,11 @@
     </row>
     <row r="119" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A119" s="57">
-        <f>A118+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B119" s="57">
-        <v>7</v>
+      <c r="B119" s="57" t="s">
+        <v>185</v>
       </c>
       <c r="C119" s="68" t="s">
         <v>11</v>
@@ -6217,8 +6310,8 @@
       <c r="A121" s="57">
         <v>9</v>
       </c>
-      <c r="B121" s="57">
-        <v>8</v>
+      <c r="B121" s="57" t="s">
+        <v>186</v>
       </c>
       <c r="C121" s="68" t="s">
         <v>174</v>
@@ -6253,8 +6346,8 @@
       <c r="A122" s="57">
         <v>10</v>
       </c>
-      <c r="B122" s="57">
-        <v>9</v>
+      <c r="B122" s="57" t="s">
+        <v>187</v>
       </c>
       <c r="C122" s="68" t="s">
         <v>174</v>
@@ -6291,8 +6384,8 @@
       <c r="A123" s="57">
         <v>11</v>
       </c>
-      <c r="B123" s="57">
-        <v>10</v>
+      <c r="B123" s="57" t="s">
+        <v>188</v>
       </c>
       <c r="C123" s="68" t="s">
         <v>174</v>
@@ -6327,8 +6420,8 @@
       <c r="A124" s="57">
         <v>12</v>
       </c>
-      <c r="B124" s="57">
-        <v>11</v>
+      <c r="B124" s="57" t="s">
+        <v>189</v>
       </c>
       <c r="C124" s="68" t="s">
         <v>174</v>
@@ -6364,8 +6457,8 @@
         <f>A124+1</f>
         <v>13</v>
       </c>
-      <c r="B125" s="57">
-        <v>12</v>
+      <c r="B125" s="57" t="s">
+        <v>190</v>
       </c>
       <c r="C125" s="68" t="s">
         <v>174</v>
@@ -6401,8 +6494,8 @@
         <f>A125+1</f>
         <v>14</v>
       </c>
-      <c r="B126" s="57">
-        <v>13</v>
+      <c r="B126" s="57" t="s">
+        <v>191</v>
       </c>
       <c r="C126" s="68" t="s">
         <v>174</v>
@@ -6438,8 +6531,8 @@
         <f>A126+1</f>
         <v>15</v>
       </c>
-      <c r="B127" s="57">
-        <v>14</v>
+      <c r="B127" s="57" t="s">
+        <v>192</v>
       </c>
       <c r="C127" s="68" t="s">
         <v>174</v>
@@ -6475,8 +6568,8 @@
         <f>A127+1</f>
         <v>16</v>
       </c>
-      <c r="B128" s="57">
-        <v>15</v>
+      <c r="B128" s="57" t="s">
+        <v>193</v>
       </c>
       <c r="C128" s="68" t="s">
         <v>174</v>
@@ -6525,11 +6618,11 @@
     </row>
     <row r="130" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A130" s="57">
-        <f>A129+1</f>
+        <f t="shared" ref="A130:A137" si="1">A129+1</f>
         <v>18</v>
       </c>
-      <c r="B130" s="57">
-        <v>16</v>
+      <c r="B130" s="57" t="s">
+        <v>194</v>
       </c>
       <c r="C130" s="68" t="s">
         <v>63</v>
@@ -6562,11 +6655,11 @@
     </row>
     <row r="131" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A131" s="57">
-        <f>A130+1</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B131" s="57">
-        <v>17</v>
+      <c r="B131" s="57" t="s">
+        <v>195</v>
       </c>
       <c r="C131" s="68" t="s">
         <v>63</v>
@@ -6601,11 +6694,11 @@
     </row>
     <row r="132" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A132" s="57">
-        <f>A131+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B132" s="57">
-        <v>18</v>
+      <c r="B132" s="57" t="s">
+        <v>196</v>
       </c>
       <c r="C132" s="68" t="s">
         <v>63</v>
@@ -6640,11 +6733,11 @@
     </row>
     <row r="133" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A133" s="57">
-        <f>A132+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B133" s="57">
-        <v>19</v>
+      <c r="B133" s="57" t="s">
+        <v>197</v>
       </c>
       <c r="C133" s="68" t="s">
         <v>63</v>
@@ -6677,11 +6770,11 @@
     </row>
     <row r="134" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A134" s="57">
-        <f>A133+1</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B134" s="57">
-        <v>20</v>
+      <c r="B134" s="57" t="s">
+        <v>198</v>
       </c>
       <c r="C134" s="68" t="s">
         <v>63</v>
@@ -6716,11 +6809,11 @@
     </row>
     <row r="135" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A135" s="57">
-        <f>A134+1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B135" s="79">
-        <v>21</v>
+      <c r="B135" s="79" t="s">
+        <v>199</v>
       </c>
       <c r="C135" s="71" t="s">
         <v>63</v>
@@ -6753,11 +6846,11 @@
     </row>
     <row r="136" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A136" s="57">
-        <f>A135+1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B136" s="79">
-        <v>22</v>
+      <c r="B136" s="79" t="s">
+        <v>200</v>
       </c>
       <c r="C136" s="71" t="s">
         <v>63</v>
@@ -6790,11 +6883,11 @@
     </row>
     <row r="137" spans="1:12" s="73" customFormat="1" ht="29.45" customHeight="1">
       <c r="A137" s="57">
-        <f>A136+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B137" s="79">
-        <v>23</v>
+      <c r="B137" s="79" t="s">
+        <v>201</v>
       </c>
       <c r="C137" s="71" t="s">
         <v>63</v>
@@ -6843,11 +6936,11 @@
     </row>
     <row r="139" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A139" s="57">
-        <f>A138+1</f>
+        <f t="shared" ref="A139:A146" si="2">A138+1</f>
         <v>27</v>
       </c>
-      <c r="B139" s="79">
-        <v>24</v>
+      <c r="B139" s="79" t="s">
+        <v>202</v>
       </c>
       <c r="C139" s="68" t="s">
         <v>77</v>
@@ -6880,11 +6973,11 @@
     </row>
     <row r="140" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A140" s="57">
-        <f>A139+1</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B140" s="79">
-        <v>25</v>
+      <c r="B140" s="79" t="s">
+        <v>203</v>
       </c>
       <c r="C140" s="68" t="s">
         <v>77</v>
@@ -6917,11 +7010,11 @@
     </row>
     <row r="141" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A141" s="57">
-        <f>A140+1</f>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="B141" s="79">
-        <v>26</v>
+      <c r="B141" s="79" t="s">
+        <v>204</v>
       </c>
       <c r="C141" s="68" t="s">
         <v>77</v>
@@ -6954,11 +7047,11 @@
     </row>
     <row r="142" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A142" s="57">
-        <f>A141+1</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B142" s="79">
-        <v>27</v>
+      <c r="B142" s="79" t="s">
+        <v>205</v>
       </c>
       <c r="C142" s="68" t="s">
         <v>77</v>
@@ -6991,11 +7084,11 @@
     </row>
     <row r="143" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A143" s="57">
-        <f>A142+1</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="B143" s="79">
-        <v>28</v>
+      <c r="B143" s="79" t="s">
+        <v>206</v>
       </c>
       <c r="C143" s="68" t="s">
         <v>77</v>
@@ -7018,21 +7111,21 @@
       <c r="I143" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="J143" s="109" t="s">
+      <c r="J143" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="K143" s="109" t="s">
+      <c r="K143" s="98" t="s">
         <v>173</v>
       </c>
       <c r="L143" s="83"/>
     </row>
     <row r="144" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A144" s="57">
-        <f>A143+1</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B144" s="79">
-        <v>29</v>
+      <c r="B144" s="79" t="s">
+        <v>207</v>
       </c>
       <c r="C144" s="68" t="s">
         <v>77</v>
@@ -7067,11 +7160,11 @@
     </row>
     <row r="145" spans="1:12" s="69" customFormat="1" ht="29.45" customHeight="1">
       <c r="A145" s="57">
-        <f>A144+1</f>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B145" s="79">
-        <v>30</v>
+      <c r="B145" s="79" t="s">
+        <v>208</v>
       </c>
       <c r="C145" s="68" t="s">
         <v>77</v>
@@ -7094,7 +7187,7 @@
       <c r="I145" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="J145" s="107" t="s">
+      <c r="J145" s="96" t="s">
         <v>15</v>
       </c>
       <c r="K145" s="93" t="s">
@@ -7104,11 +7197,11 @@
     </row>
     <row r="146" spans="1:12" ht="30">
       <c r="A146" s="57">
-        <f>A145+1</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="B146" s="86">
-        <v>31</v>
+      <c r="B146" s="86" t="s">
+        <v>209</v>
       </c>
       <c r="C146" s="87" t="s">
         <v>77</v>
@@ -7122,7 +7215,7 @@
       <c r="F146" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="G146" s="106" t="s">
+      <c r="G146" s="95" t="s">
         <v>167</v>
       </c>
       <c r="H146" s="89" t="s">
@@ -7134,7 +7227,7 @@
       <c r="J146" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="K146" s="108" t="s">
+      <c r="K146" s="97" t="s">
         <v>171</v>
       </c>
       <c r="L146" s="92"/>

</xml_diff>

<commit_message>
Excel to CCSL (2/4)
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6637D499-D487-4DE6-9E68-132D195B97FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC3229-6F54-4F1D-9EE7-6C1326E266E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K125" sqref="K125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Excel to CCSL (100%)
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAC3229-6F54-4F1D-9EE7-6C1326E266E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0064F5A3-DDA0-4FE5-8507-7DE2C1F85B85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K125" sqref="K125"/>
+    <sheetView tabSelected="1" topLeftCell="B130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Ajout Commentaire pour Trigger
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0064F5A3-DDA0-4FE5-8507-7DE2C1F85B85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF462AB-855E-427E-B93A-F562C05C5722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:AB151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I146" sqref="I146"/>
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Table de transition avec toutes les variables
Quantité d'inconnues impressionnante!
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\TERS2\TER_SafetyCriticalSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\S2\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF462AB-855E-427E-B93A-F562C05C5722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57115051-8D98-4A3F-98AA-EC12CE240DD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="C130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Rapport PDF V3, Fix Recurrence, XML, and more
</commit_message>
<xml_diff>
--- a/Matrix-Usecase-V1.xlsx
+++ b/Matrix-Usecase-V1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\S2\TERS2\TER_SafetyCriticalSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57115051-8D98-4A3F-98AA-EC12CE240DD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC33205E-B5CA-4584-97FA-205BF5FD6CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
 </workbook>
 </file>
 
@@ -1872,8 +1872,8 @@
   </sheetPr>
   <dimension ref="A1:AB151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H115" sqref="H115"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -6219,7 +6219,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B118" s="59" t="s">
+      <c r="B118" s="57" t="s">
         <v>184</v>
       </c>
       <c r="C118" s="68" t="s">

</xml_diff>